<commit_message>
Adding fridge and testing the cat animations
</commit_message>
<xml_diff>
--- a/research/Animals.xlsx
+++ b/research/Animals.xlsx
@@ -1,18 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
   <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JarvisWalker/Documents/Git/JSPets/research/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="21620" windowHeight="12640" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="88">
   <si>
     <t>City</t>
   </si>
@@ -281,13 +292,16 @@
   </si>
   <si>
     <t>Attack modifier</t>
+  </si>
+  <si>
+    <t>Modifiers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -331,8 +345,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -357,6 +378,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
       </patternFill>
     </fill>
   </fills>
@@ -384,36 +410,39 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="5"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
+    <cellStyle name="Accent5" xfId="5" builtinId="45"/>
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Input" xfId="4" builtinId="20"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="30">
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -474,6 +503,236 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -762,13 +1021,13 @@
       <selection pane="bottomRight" activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="61.42578125" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="61.5" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -809,7 +1068,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -827,7 +1086,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -845,7 +1104,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -860,7 +1119,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -881,7 +1140,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -902,7 +1161,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -920,7 +1179,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -938,7 +1197,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -950,7 +1209,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -968,7 +1227,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -986,7 +1245,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1004,7 +1263,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1025,7 +1284,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1040,7 +1299,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1058,7 +1317,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1073,7 +1332,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1091,7 +1350,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1109,7 +1368,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1130,7 +1389,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>70</v>
       </c>
@@ -1181,7 +1440,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B19">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="27" priority="1" operator="lessThan">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1192,46 +1451,48 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X37"/>
+  <dimension ref="A1:AA37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L3" sqref="L3"/>
+      <selection pane="bottomRight" activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" customWidth="1"/>
+    <col min="1" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" customWidth="1"/>
+    <col min="14" max="14" width="11.6640625" customWidth="1"/>
+    <col min="15" max="15" width="12.83203125" customWidth="1"/>
+    <col min="16" max="16" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="E1" s="3" t="s">
+    <row r="1" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="E1" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
       <c r="S1" s="4"/>
       <c r="T1" s="4"/>
@@ -1239,8 +1500,11 @@
       <c r="V1" s="4"/>
       <c r="W1" s="4"/>
       <c r="X1" s="4"/>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4"/>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -1272,49 +1536,58 @@
         <v>65</v>
       </c>
       <c r="K2" t="s">
+        <v>63</v>
+      </c>
+      <c r="L2" t="s">
+        <v>64</v>
+      </c>
+      <c r="M2" t="s">
+        <v>65</v>
+      </c>
+      <c r="N2" t="s">
         <v>79</v>
       </c>
-      <c r="L2" t="s">
+      <c r="O2" t="s">
         <v>80</v>
       </c>
-      <c r="M2" t="s">
+      <c r="P2" t="s">
         <v>81</v>
       </c>
-      <c r="N2" t="s">
+      <c r="Q2" t="s">
         <v>19</v>
       </c>
-      <c r="O2" t="s">
+      <c r="R2" t="s">
         <v>20</v>
       </c>
-      <c r="P2" t="s">
+      <c r="S2" t="s">
         <v>21</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="T2" t="s">
         <v>22</v>
       </c>
-      <c r="R2" t="s">
+      <c r="U2" t="s">
         <v>23</v>
       </c>
-      <c r="S2" t="s">
+      <c r="V2" t="s">
         <v>24</v>
       </c>
-      <c r="T2" t="s">
+      <c r="W2" t="s">
         <v>25</v>
       </c>
-      <c r="U2" t="s">
+      <c r="X2" t="s">
         <v>26</v>
       </c>
-      <c r="V2" t="s">
+      <c r="Y2" t="s">
         <v>27</v>
       </c>
-      <c r="W2" t="s">
+      <c r="Z2" t="s">
         <v>28</v>
       </c>
-      <c r="X2" t="s">
+      <c r="AA2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1325,21 +1598,37 @@
         <v>2</v>
       </c>
       <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
         <v>9</v>
       </c>
-      <c r="F3">
+      <c r="I3">
+        <v>4</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <f>H3*D3*E3</f>
+        <v>18</v>
+      </c>
+      <c r="L3">
+        <f>I3*F3*D3</f>
         <v>8</v>
       </c>
-      <c r="H3">
-        <f>E3*D3</f>
-        <v>18</v>
-      </c>
-      <c r="I3">
-        <f>ROUNDUP(F3*1.4,0)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="M3">
+        <f>(J3+G3)*D3</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -1350,14 +1639,34 @@
         <v>2</v>
       </c>
       <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
         <v>15</v>
       </c>
-      <c r="H4">
-        <f t="shared" ref="H4:H37" si="0">E4*D4</f>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <f t="shared" ref="K4:K37" si="0">H4*D4*E4</f>
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <f t="shared" ref="L4:L37" si="1">I4*F4*D4</f>
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <f t="shared" ref="M4:M37" si="2">(J4+G4)*D4</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -1368,14 +1677,34 @@
         <v>2</v>
       </c>
       <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
         <v>36</v>
       </c>
-      <c r="H5">
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -1386,14 +1715,34 @@
         <v>3</v>
       </c>
       <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
         <v>8</v>
       </c>
-      <c r="H6">
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1404,14 +1753,34 @@
         <v>2</v>
       </c>
       <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
         <v>7</v>
       </c>
-      <c r="H7">
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -1422,14 +1791,46 @@
         <v>2</v>
       </c>
       <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
         <v>9</v>
       </c>
-      <c r="H8">
+      <c r="I8">
+        <v>4</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+      <c r="L8">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="N8">
+        <v>0.3</v>
+      </c>
+      <c r="O8">
+        <v>0.6</v>
+      </c>
+      <c r="Y8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>46</v>
       </c>
@@ -1440,14 +1841,34 @@
         <v>2</v>
       </c>
       <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
         <v>8</v>
       </c>
-      <c r="H9">
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -1458,14 +1879,34 @@
         <v>2</v>
       </c>
       <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
         <v>10</v>
       </c>
-      <c r="H10">
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="L10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -1476,14 +1917,34 @@
         <v>2</v>
       </c>
       <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
         <v>8</v>
       </c>
-      <c r="H11">
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="L11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -1494,14 +1955,34 @@
         <v>3</v>
       </c>
       <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
         <v>6</v>
       </c>
-      <c r="H12">
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="L12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -1512,14 +1993,34 @@
         <v>3</v>
       </c>
       <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
         <v>7</v>
       </c>
-      <c r="H13">
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="L13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -1530,14 +2031,34 @@
         <v>2</v>
       </c>
       <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
         <v>6</v>
       </c>
-      <c r="H14">
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+      <c r="L14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>41</v>
       </c>
@@ -1545,14 +2066,34 @@
         <v>72</v>
       </c>
       <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
         <v>8</v>
       </c>
-      <c r="H15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -1563,14 +2104,34 @@
         <v>3</v>
       </c>
       <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
         <v>12</v>
       </c>
-      <c r="H16">
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -1581,14 +2142,34 @@
         <v>2</v>
       </c>
       <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
         <v>8</v>
       </c>
-      <c r="H17">
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -1599,14 +2180,34 @@
         <v>3</v>
       </c>
       <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>0.5</v>
+      </c>
+      <c r="H18">
         <v>10</v>
       </c>
-      <c r="H18">
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="2"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>45</v>
       </c>
@@ -1617,14 +2218,34 @@
         <v>3</v>
       </c>
       <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
         <v>8</v>
       </c>
-      <c r="H19">
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -1635,14 +2256,34 @@
         <v>3</v>
       </c>
       <c r="E20">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
       </c>
       <c r="H20">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -1653,14 +2294,34 @@
         <v>3</v>
       </c>
       <c r="E21">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
       </c>
       <c r="H21">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -1671,14 +2332,52 @@
         <v>3</v>
       </c>
       <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
         <v>8</v>
       </c>
-      <c r="H22">
+      <c r="I22">
+        <v>4</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="L22">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="N22">
+        <v>0.4</v>
+      </c>
+      <c r="O22">
+        <v>0.7</v>
+      </c>
+      <c r="Q22">
+        <v>5</v>
+      </c>
+      <c r="U22">
+        <v>10</v>
+      </c>
+      <c r="AA22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>52</v>
       </c>
@@ -1686,14 +2385,34 @@
         <v>73</v>
       </c>
       <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
         <v>8</v>
       </c>
-      <c r="H23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>53</v>
       </c>
@@ -1704,14 +2423,34 @@
         <v>3</v>
       </c>
       <c r="E24">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
       </c>
       <c r="H24">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>54</v>
       </c>
@@ -1722,14 +2461,34 @@
         <v>3</v>
       </c>
       <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25">
         <v>8</v>
       </c>
-      <c r="H25">
+      <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="K25">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>55</v>
       </c>
@@ -1740,14 +2499,34 @@
         <v>3</v>
       </c>
       <c r="E26">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
       </c>
       <c r="H26">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>56</v>
       </c>
@@ -1758,14 +2537,34 @@
         <v>3</v>
       </c>
       <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
         <v>8</v>
       </c>
-      <c r="H27">
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>57</v>
       </c>
@@ -1776,14 +2575,34 @@
         <v>3</v>
       </c>
       <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
         <v>8</v>
       </c>
-      <c r="H28">
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>58</v>
       </c>
@@ -1794,14 +2613,34 @@
         <v>3</v>
       </c>
       <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
         <v>8</v>
       </c>
-      <c r="H29">
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="K29">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>59</v>
       </c>
@@ -1812,14 +2651,34 @@
         <v>3</v>
       </c>
       <c r="E30">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
       </c>
       <c r="H30">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>60</v>
       </c>
@@ -1830,14 +2689,34 @@
         <v>2</v>
       </c>
       <c r="E31">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
       </c>
       <c r="H31">
-        <f t="shared" si="0"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J31">
+        <v>1</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>61</v>
       </c>
@@ -1848,14 +2727,34 @@
         <v>3</v>
       </c>
       <c r="E32">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
       </c>
       <c r="H32">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="J32">
+        <v>1</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>77</v>
       </c>
@@ -1866,14 +2765,34 @@
         <v>2</v>
       </c>
       <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33">
         <v>8</v>
       </c>
-      <c r="H33">
+      <c r="J33">
+        <v>1</v>
+      </c>
+      <c r="K33">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>62</v>
       </c>
@@ -1884,14 +2803,34 @@
         <v>3</v>
       </c>
       <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34">
         <v>8</v>
       </c>
-      <c r="H34">
+      <c r="J34">
+        <v>1</v>
+      </c>
+      <c r="K34">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>82</v>
       </c>
@@ -1902,14 +2841,34 @@
         <v>1</v>
       </c>
       <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="H35">
         <v>36</v>
       </c>
-      <c r="H35">
+      <c r="J35">
+        <v>1</v>
+      </c>
+      <c r="K35">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>83</v>
       </c>
@@ -1920,14 +2879,37 @@
         <v>1</v>
       </c>
       <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36">
         <v>80</v>
       </c>
-      <c r="H36">
+      <c r="I36">
+        <v>10</v>
+      </c>
+      <c r="J36">
+        <v>1</v>
+      </c>
+      <c r="K36">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L36">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>85</v>
       </c>
@@ -1938,31 +2920,54 @@
         <v>1</v>
       </c>
       <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+      <c r="H37">
         <v>20</v>
       </c>
-      <c r="H37">
+      <c r="J37">
+        <v>1</v>
+      </c>
+      <c r="K37">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
+      <c r="L37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="top10" dxfId="5" priority="6" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="top10" dxfId="4" priority="5" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="top10" dxfId="3" priority="4" rank="10"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="top10" dxfId="2" priority="3" rank="10"/>
+    <cfRule type="top10" dxfId="21" priority="3" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="20" priority="10" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="top10" dxfId="1" priority="2" rank="10"/>
+    <cfRule type="top10" dxfId="19" priority="9" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J1:M1048576">
-    <cfRule type="top10" dxfId="0" priority="1" rank="10"/>
+  <conditionalFormatting sqref="K1:K1048576">
+    <cfRule type="top10" dxfId="18" priority="4" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="17" priority="7" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L1:L1048576">
+    <cfRule type="top10" dxfId="16" priority="6" rank="10"/>
+    <cfRule type="top10" dxfId="15" priority="2" bottom="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M1:P1048576">
+    <cfRule type="top10" dxfId="14" priority="5" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J1:J1048576">
+    <cfRule type="top10" dxfId="4" priority="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Updating the spawn rates
</commit_message>
<xml_diff>
--- a/research/Animals.xlsx
+++ b/research/Animals.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="21620" windowHeight="12640" activeTab="1"/>
+    <workbookView xWindow="5120" yWindow="1920" windowWidth="23080" windowHeight="12640" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="89">
   <si>
     <t>City</t>
   </si>
@@ -295,6 +295,9 @@
   </si>
   <si>
     <t>Modifiers</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -435,17 +438,7 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -453,126 +446,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -658,81 +531,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1015,10 +818,10 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J20" sqref="J20"/>
+      <selection pane="bottomRight" activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1440,7 +1243,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B19">
-    <cfRule type="cellIs" dxfId="27" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="lessThan">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1451,13 +1254,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA37"/>
+  <dimension ref="A1:AA41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="O18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I35" sqref="I35"/>
+      <selection pane="bottomRight" activeCell="Q43" sqref="Q43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1627,6 +1430,18 @@
         <f>(J3+G3)*D3</f>
         <v>4</v>
       </c>
+      <c r="R3">
+        <v>10</v>
+      </c>
+      <c r="S3">
+        <v>10</v>
+      </c>
+      <c r="W3">
+        <v>10</v>
+      </c>
+      <c r="Y3">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -1665,6 +1480,9 @@
         <f t="shared" ref="M4:M37" si="2">(J4+G4)*D4</f>
         <v>4</v>
       </c>
+      <c r="T4">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -1703,6 +1521,9 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
+      <c r="U5">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -1741,6 +1562,12 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
+      <c r="S6">
+        <v>10</v>
+      </c>
+      <c r="V6">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -1779,6 +1606,9 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
+      <c r="Y7">
+        <v>10</v>
+      </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -1821,10 +1651,10 @@
         <v>4</v>
       </c>
       <c r="N8">
-        <v>0.3</v>
+        <v>3</v>
       </c>
       <c r="O8">
-        <v>0.6</v>
+        <v>6</v>
       </c>
       <c r="Y8">
         <v>10</v>
@@ -1868,7 +1698,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -1943,6 +1773,18 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
+      <c r="R11">
+        <v>2</v>
+      </c>
+      <c r="S11">
+        <v>10</v>
+      </c>
+      <c r="U11">
+        <v>10</v>
+      </c>
+      <c r="AA11">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -1981,6 +1823,18 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
+      <c r="S12">
+        <v>8</v>
+      </c>
+      <c r="V12">
+        <v>6</v>
+      </c>
+      <c r="W12">
+        <v>3</v>
+      </c>
+      <c r="X12">
+        <v>8</v>
+      </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -2019,6 +1873,18 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
+      <c r="R13">
+        <v>1</v>
+      </c>
+      <c r="S13">
+        <v>10</v>
+      </c>
+      <c r="V13">
+        <v>8</v>
+      </c>
+      <c r="AA13">
+        <v>8</v>
+      </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -2057,6 +1923,15 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
+      <c r="S14">
+        <v>10</v>
+      </c>
+      <c r="W14">
+        <v>3</v>
+      </c>
+      <c r="Y14">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
@@ -2130,6 +2005,12 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
+      <c r="Q16">
+        <v>8</v>
+      </c>
+      <c r="R16">
+        <v>8</v>
+      </c>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -2168,6 +2049,24 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
+      <c r="R17">
+        <v>10</v>
+      </c>
+      <c r="S17">
+        <v>8</v>
+      </c>
+      <c r="V17">
+        <v>10</v>
+      </c>
+      <c r="Y17">
+        <v>10</v>
+      </c>
+      <c r="Z17">
+        <v>10</v>
+      </c>
+      <c r="AA17">
+        <v>8</v>
+      </c>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
@@ -2206,6 +2105,9 @@
         <f t="shared" si="2"/>
         <v>4.5</v>
       </c>
+      <c r="AA18">
+        <v>10</v>
+      </c>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
@@ -2244,6 +2146,9 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
+      <c r="T19">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
@@ -2282,6 +2187,12 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
+      <c r="Q20">
+        <v>4</v>
+      </c>
+      <c r="R20">
+        <v>6</v>
+      </c>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
@@ -2320,6 +2231,18 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
+      <c r="Q21">
+        <v>10</v>
+      </c>
+      <c r="R21">
+        <v>10</v>
+      </c>
+      <c r="U21">
+        <v>3</v>
+      </c>
+      <c r="AA21">
+        <v>6</v>
+      </c>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
@@ -2362,10 +2285,10 @@
         <v>6</v>
       </c>
       <c r="N22">
-        <v>0.4</v>
+        <v>4</v>
       </c>
       <c r="O22">
-        <v>0.7</v>
+        <v>7</v>
       </c>
       <c r="Q22">
         <v>5</v>
@@ -2412,7 +2335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>53</v>
       </c>
@@ -2448,6 +2371,39 @@
       <c r="M24">
         <f t="shared" si="2"/>
         <v>6</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>88</v>
+      </c>
+      <c r="R24" t="s">
+        <v>88</v>
+      </c>
+      <c r="S24" t="s">
+        <v>88</v>
+      </c>
+      <c r="T24" t="s">
+        <v>88</v>
+      </c>
+      <c r="U24" t="s">
+        <v>88</v>
+      </c>
+      <c r="V24" t="s">
+        <v>88</v>
+      </c>
+      <c r="W24" t="s">
+        <v>88</v>
+      </c>
+      <c r="X24" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
@@ -2487,6 +2443,9 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
+      <c r="Q25" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
@@ -2525,6 +2484,15 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
+      <c r="R26">
+        <v>10</v>
+      </c>
+      <c r="Y26">
+        <v>10</v>
+      </c>
+      <c r="Z26">
+        <v>10</v>
+      </c>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
@@ -2563,6 +2531,18 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
+      <c r="S27">
+        <v>5</v>
+      </c>
+      <c r="V27">
+        <v>10</v>
+      </c>
+      <c r="Y27">
+        <v>10</v>
+      </c>
+      <c r="Z27">
+        <v>10</v>
+      </c>
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
@@ -2601,6 +2581,15 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
+      <c r="S28">
+        <v>10</v>
+      </c>
+      <c r="V28">
+        <v>5</v>
+      </c>
+      <c r="Z28">
+        <v>5</v>
+      </c>
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
@@ -2639,6 +2628,21 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
+      <c r="S29">
+        <v>10</v>
+      </c>
+      <c r="V29">
+        <v>5</v>
+      </c>
+      <c r="Y29">
+        <v>5</v>
+      </c>
+      <c r="Z29">
+        <v>8</v>
+      </c>
+      <c r="AA29">
+        <v>3</v>
+      </c>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
@@ -2677,6 +2681,15 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
+      <c r="S30">
+        <v>3</v>
+      </c>
+      <c r="W30">
+        <v>3</v>
+      </c>
+      <c r="X30">
+        <v>3</v>
+      </c>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
@@ -2715,6 +2728,9 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
+      <c r="T31">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
@@ -2753,8 +2769,14 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="U32">
+        <v>10</v>
+      </c>
+      <c r="AA32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>77</v>
       </c>
@@ -2791,8 +2813,17 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="S33">
+        <v>3</v>
+      </c>
+      <c r="Z33">
+        <v>3</v>
+      </c>
+      <c r="AA33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>62</v>
       </c>
@@ -2829,8 +2860,14 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="V34">
+        <v>10</v>
+      </c>
+      <c r="Z34">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>82</v>
       </c>
@@ -2867,8 +2904,11 @@
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="X35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>83</v>
       </c>
@@ -2908,8 +2948,14 @@
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N36">
+        <v>5</v>
+      </c>
+      <c r="W36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>85</v>
       </c>
@@ -2946,28 +2992,126 @@
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
+      <c r="Q37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q40">
+        <f>COUNT(Q3:Q39)</f>
+        <v>5</v>
+      </c>
+      <c r="R40">
+        <f t="shared" ref="R40:AA40" si="3">COUNT(R3:R39)</f>
+        <v>8</v>
+      </c>
+      <c r="S40">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="T40">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="U40">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="V40">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="W40">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="X40">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="Y40">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="Z40">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="AA40">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="Q41">
+        <f>SUM(Q3:Q39)</f>
+        <v>30</v>
+      </c>
+      <c r="R41">
+        <f t="shared" ref="R41:AA41" si="4">SUM(R3:R39)</f>
+        <v>57</v>
+      </c>
+      <c r="S41">
+        <f t="shared" si="4"/>
+        <v>97</v>
+      </c>
+      <c r="T41">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="U41">
+        <f t="shared" si="4"/>
+        <v>38</v>
+      </c>
+      <c r="V41">
+        <f t="shared" si="4"/>
+        <v>62</v>
+      </c>
+      <c r="W41">
+        <f t="shared" si="4"/>
+        <v>22</v>
+      </c>
+      <c r="X41">
+        <f t="shared" si="4"/>
+        <v>21</v>
+      </c>
+      <c r="Y41">
+        <f t="shared" si="4"/>
+        <v>60</v>
+      </c>
+      <c r="Z41">
+        <f t="shared" si="4"/>
+        <v>56</v>
+      </c>
+      <c r="AA41">
+        <f t="shared" si="4"/>
+        <v>63</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="top10" dxfId="21" priority="3" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="20" priority="10" rank="10"/>
+    <cfRule type="top10" dxfId="8" priority="3" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="7" priority="10" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="top10" dxfId="19" priority="9" rank="10"/>
+    <cfRule type="top10" dxfId="6" priority="9" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="top10" dxfId="18" priority="4" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="17" priority="7" rank="10"/>
+    <cfRule type="top10" dxfId="5" priority="4" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="4" priority="7" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="top10" dxfId="16" priority="6" rank="10"/>
-    <cfRule type="top10" dxfId="15" priority="2" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="3" priority="6" rank="10"/>
+    <cfRule type="top10" dxfId="2" priority="2" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:P1048576">
-    <cfRule type="top10" dxfId="14" priority="5" rank="10"/>
+    <cfRule type="top10" dxfId="1" priority="5" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="top10" dxfId="4" priority="1" rank="10"/>
+    <cfRule type="top10" dxfId="0" priority="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Splitting some of the logic out
</commit_message>
<xml_diff>
--- a/research/Animals.xlsx
+++ b/research/Animals.xlsx
@@ -1,37 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
   <workbookPr filterPrivacy="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JarvisWalker/Documents/Git/JSPets/research/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5120" yWindow="1920" windowWidth="23080" windowHeight="12640" activeTab="1"/>
+    <workbookView xWindow="5115" yWindow="1920" windowWidth="23085" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="90">
   <si>
     <t>City</t>
   </si>
@@ -298,12 +293,15 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>How do I get this number?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -824,13 +822,13 @@
       <selection pane="bottomRight" activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="61.5" customWidth="1"/>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="1" max="1" width="61.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -871,7 +869,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -889,7 +887,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -907,7 +905,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -922,7 +920,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -943,7 +941,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -964,7 +962,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -982,7 +980,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1000,7 +998,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1012,7 +1010,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1030,7 +1028,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1048,7 +1046,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1066,7 +1064,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1087,7 +1085,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1102,7 +1100,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1120,7 +1118,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1135,7 +1133,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1153,7 +1151,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1171,7 +1169,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1192,7 +1190,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>70</v>
       </c>
@@ -1254,25 +1252,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA41"/>
+  <dimension ref="A1:AC48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="O18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="O17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q43" sqref="Q43"/>
+      <selection pane="bottomRight" activeCell="AC42" sqref="AC42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="17.5" customWidth="1"/>
-    <col min="3" max="3" width="16.1640625" customWidth="1"/>
-    <col min="14" max="14" width="11.6640625" customWidth="1"/>
-    <col min="15" max="15" width="12.83203125" customWidth="1"/>
-    <col min="16" max="16" width="14.5" customWidth="1"/>
+    <col min="1" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E1" s="6" t="s">
         <v>87</v>
       </c>
@@ -1307,7 +1305,7 @@
       <c r="Z1" s="4"/>
       <c r="AA1" s="4"/>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -1390,7 +1388,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1443,7 +1441,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -1484,7 +1482,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -1525,7 +1523,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -1569,7 +1567,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1610,7 +1608,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -1660,7 +1658,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>46</v>
       </c>
@@ -1698,7 +1696,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -1736,7 +1734,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -1786,7 +1784,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -1836,7 +1834,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -1886,7 +1884,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -1933,7 +1931,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>41</v>
       </c>
@@ -1968,7 +1966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -2012,7 +2010,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -2068,7 +2066,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -2109,7 +2107,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>45</v>
       </c>
@@ -2150,7 +2148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -2194,7 +2192,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -2244,7 +2242,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -2300,7 +2298,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>52</v>
       </c>
@@ -2335,7 +2333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>53</v>
       </c>
@@ -2406,7 +2404,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>54</v>
       </c>
@@ -2447,7 +2445,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>55</v>
       </c>
@@ -2494,7 +2492,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>56</v>
       </c>
@@ -2544,7 +2542,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>57</v>
       </c>
@@ -2591,7 +2589,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>58</v>
       </c>
@@ -2644,7 +2642,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>59</v>
       </c>
@@ -2691,7 +2689,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>60</v>
       </c>
@@ -2732,7 +2730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>61</v>
       </c>
@@ -2776,7 +2774,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>77</v>
       </c>
@@ -2823,7 +2821,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>62</v>
       </c>
@@ -2867,7 +2865,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>82</v>
       </c>
@@ -2908,7 +2906,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>83</v>
       </c>
@@ -2955,7 +2953,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>85</v>
       </c>
@@ -2996,7 +2994,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>70</v>
       </c>
@@ -3045,7 +3043,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
       <c r="Q41">
         <f>SUM(Q3:Q39)</f>
         <v>30</v>
@@ -3089,6 +3087,45 @@
       <c r="AA41">
         <f t="shared" si="4"/>
         <v>63</v>
+      </c>
+      <c r="AC41" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Q43">
+        <f>Q37/Q41</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Q44">
+        <f>Q22/Q41</f>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="45" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Q45">
+        <f>Q21/Q41</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Q46">
+        <f>Q20/Q41</f>
+        <v>0.13333333333333333</v>
+      </c>
+    </row>
+    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Q47">
+        <f>Q16/Q41</f>
+        <v>0.26666666666666666</v>
+      </c>
+    </row>
+    <row r="48" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Q48">
+        <f xml:space="preserve"> SUM(Q43:Q47)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Starting to fill in the biome generation code, from here, look at adding the animals into each biome
</commit_message>
<xml_diff>
--- a/research/Animals.xlsx
+++ b/research/Animals.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="1920" windowWidth="23085" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="5115" yWindow="1920" windowWidth="23085" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="93">
   <si>
     <t>City</t>
   </si>
@@ -296,6 +296,15 @@
   </si>
   <si>
     <t>How do I get this number?</t>
+  </si>
+  <si>
+    <t>Alpine</t>
+  </si>
+  <si>
+    <t>grasslands</t>
+  </si>
+  <si>
+    <t>plains</t>
   </si>
 </sst>
 </file>
@@ -815,17 +824,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L16" sqref="L16"/>
+      <selection pane="bottomRight" activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="61.42578125" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="4.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -851,19 +861,19 @@
         <v>23</v>
       </c>
       <c r="H1" t="s">
-        <v>24</v>
+        <v>91</v>
       </c>
       <c r="I1" t="s">
         <v>25</v>
       </c>
       <c r="J1" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="K1" t="s">
         <v>27</v>
       </c>
       <c r="L1" t="s">
-        <v>28</v>
+        <v>92</v>
       </c>
       <c r="M1" t="s">
         <v>29</v>
@@ -1159,11 +1169,14 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
+      <c r="C18">
+        <v>20</v>
+      </c>
       <c r="D18">
         <v>30</v>
       </c>
       <c r="K18">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="M18">
         <v>30</v>
@@ -1196,7 +1209,7 @@
       </c>
       <c r="C20">
         <f>COUNTA(C2:C19)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D20">
         <f t="shared" ref="D20:M20" si="1">COUNTA(D2:D19)</f>
@@ -1254,11 +1267,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="O17" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="H5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AC42" sqref="AC42"/>
+      <selection pane="bottomRight" activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Adding in the animal typings and figuring out how to pick a biome to spawn something from
</commit_message>
<xml_diff>
--- a/research/Animals.xlsx
+++ b/research/Animals.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="1920" windowWidth="23085" windowHeight="12645"/>
+    <workbookView xWindow="5115" yWindow="1920" windowWidth="23085" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="91">
   <si>
     <t>City</t>
   </si>
@@ -100,21 +100,12 @@
     <t>5. Lakes</t>
   </si>
   <si>
-    <t>6. Plains</t>
-  </si>
-  <si>
     <t>7. Rocks</t>
   </si>
   <si>
-    <t>8. Snowy</t>
-  </si>
-  <si>
     <t>9. Urban</t>
   </si>
   <si>
-    <t>10. Valley</t>
-  </si>
-  <si>
     <t>11. Wetlands</t>
   </si>
   <si>
@@ -305,6 +296,9 @@
   </si>
   <si>
     <t>plains</t>
+  </si>
+  <si>
+    <t>Difficulty</t>
   </si>
 </sst>
 </file>
@@ -445,7 +439,57 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -523,16 +567,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -822,13 +856,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M20"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M18" sqref="M18"/>
+      <selection pane="bottomRight" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -838,12 +872,12 @@
     <col min="6" max="6" width="4.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C1" t="s">
         <v>19</v>
@@ -861,25 +895,28 @@
         <v>23</v>
       </c>
       <c r="H1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K1" t="s">
         <v>25</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
+        <v>89</v>
+      </c>
+      <c r="M1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" t="s">
         <v>90</v>
       </c>
-      <c r="K1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L1" t="s">
-        <v>92</v>
-      </c>
-      <c r="M1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -896,8 +933,11 @@
       <c r="K2">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -914,8 +954,11 @@
       <c r="K3">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -929,8 +972,11 @@
       <c r="K4">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -950,8 +996,11 @@
       <c r="M5">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -971,8 +1020,11 @@
       <c r="M6">
         <v>40</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -989,8 +1041,11 @@
       <c r="M7">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1007,8 +1062,11 @@
       <c r="H8">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N8">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1019,8 +1077,11 @@
       <c r="C9">
         <v>100</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N9">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1037,8 +1098,11 @@
       <c r="K10">
         <v>60</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N10">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1055,8 +1119,11 @@
       <c r="M11">
         <v>50</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N11">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1073,8 +1140,11 @@
       <c r="M12">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N12">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1094,8 +1164,11 @@
       <c r="L13">
         <v>30</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N13">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1109,8 +1182,11 @@
       <c r="K14">
         <v>50</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N14">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1127,8 +1203,11 @@
       <c r="M15">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N15">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1142,8 +1221,11 @@
       <c r="L16">
         <v>50</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N16">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1160,8 +1242,11 @@
       <c r="M17">
         <v>60</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N17">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1181,8 +1266,11 @@
       <c r="M18">
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1202,10 +1290,13 @@
       <c r="M19">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N19">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C20">
         <f>COUNTA(C2:C19)</f>
@@ -1254,9 +1345,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B19">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="lessThan">
       <formula>100</formula>
     </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N1:N1048576">
+    <cfRule type="top10" dxfId="2" priority="1" rank="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -1267,11 +1361,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="H5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="L3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T4" sqref="T4"/>
+      <selection pane="bottomRight" activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1285,27 +1379,27 @@
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E1" s="6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
       <c r="H1" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="O1" s="5"/>
       <c r="P1" s="5"/>
       <c r="Q1" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="R1" s="4"/>
       <c r="S1" s="4"/>
@@ -1320,52 +1414,52 @@
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="I2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="J2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="K2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="L2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="M2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="O2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="P2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="Q2" t="s">
         <v>19</v>
@@ -1383,30 +1477,30 @@
         <v>23</v>
       </c>
       <c r="V2" t="s">
+        <v>88</v>
+      </c>
+      <c r="W2" t="s">
         <v>24</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y2" t="s">
         <v>25</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Z2" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA2" t="s">
         <v>26</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -1456,10 +1550,10 @@
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -1497,10 +1591,10 @@
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -1538,10 +1632,10 @@
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D6">
         <v>3</v>
@@ -1582,10 +1676,10 @@
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -1623,10 +1717,10 @@
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -1673,10 +1767,10 @@
     </row>
     <row r="9" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -1711,10 +1805,10 @@
     </row>
     <row r="10" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D10">
         <v>2</v>
@@ -1749,10 +1843,10 @@
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -1799,10 +1893,10 @@
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D12">
         <v>3</v>
@@ -1849,10 +1943,10 @@
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D13">
         <v>3</v>
@@ -1899,10 +1993,10 @@
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -1946,10 +2040,10 @@
     </row>
     <row r="15" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B15" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -1981,10 +2075,10 @@
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B16" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D16">
         <v>3</v>
@@ -2025,10 +2119,10 @@
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B17" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D17">
         <v>2</v>
@@ -2081,10 +2175,10 @@
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D18">
         <v>3</v>
@@ -2122,10 +2216,10 @@
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B19" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D19">
         <v>3</v>
@@ -2163,10 +2257,10 @@
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B20" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D20">
         <v>3</v>
@@ -2207,10 +2301,10 @@
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B21" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D21">
         <v>3</v>
@@ -2257,10 +2351,10 @@
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B22" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D22">
         <v>3</v>
@@ -2313,10 +2407,10 @@
     </row>
     <row r="23" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B23" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -2348,10 +2442,10 @@
     </row>
     <row r="24" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B24" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D24">
         <v>3</v>
@@ -2384,45 +2478,45 @@
         <v>6</v>
       </c>
       <c r="Q24" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="R24" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="S24" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="T24" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="U24" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="V24" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="W24" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="X24" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="Y24" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="Z24" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="AA24" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B25" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D25">
         <v>3</v>
@@ -2455,15 +2549,15 @@
         <v>6</v>
       </c>
       <c r="Q25" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B26" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D26">
         <v>3</v>
@@ -2507,10 +2601,10 @@
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B27" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D27">
         <v>3</v>
@@ -2557,10 +2651,10 @@
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B28" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D28">
         <v>3</v>
@@ -2604,10 +2698,10 @@
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B29" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D29">
         <v>3</v>
@@ -2657,10 +2751,10 @@
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B30" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D30">
         <v>3</v>
@@ -2704,10 +2798,10 @@
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B31" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D31">
         <v>2</v>
@@ -2745,10 +2839,10 @@
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B32" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D32">
         <v>3</v>
@@ -2789,10 +2883,10 @@
     </row>
     <row r="33" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B33" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D33">
         <v>2</v>
@@ -2836,10 +2930,10 @@
     </row>
     <row r="34" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B34" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D34">
         <v>3</v>
@@ -2880,10 +2974,10 @@
     </row>
     <row r="35" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B35" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -2921,10 +3015,10 @@
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B36" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -2968,10 +3062,10 @@
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B37" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -3009,7 +3103,7 @@
     </row>
     <row r="40" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="Q40">
         <f>COUNT(Q3:Q39)</f>
@@ -3102,7 +3196,7 @@
         <v>63</v>
       </c>
       <c r="AC41" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="43" spans="1:29" x14ac:dyDescent="0.25">
@@ -3143,25 +3237,25 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="top10" dxfId="8" priority="3" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="7" priority="10" rank="10"/>
+    <cfRule type="top10" dxfId="13" priority="3" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="12" priority="10" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="top10" dxfId="6" priority="9" rank="10"/>
+    <cfRule type="top10" dxfId="11" priority="9" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="top10" dxfId="5" priority="4" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="4" priority="7" rank="10"/>
+    <cfRule type="top10" dxfId="10" priority="4" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="9" priority="7" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="top10" dxfId="3" priority="6" rank="10"/>
-    <cfRule type="top10" dxfId="2" priority="2" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="8" priority="6" rank="10"/>
+    <cfRule type="top10" dxfId="7" priority="2" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:P1048576">
-    <cfRule type="top10" dxfId="1" priority="5" rank="10"/>
+    <cfRule type="top10" dxfId="6" priority="5" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="top10" dxfId="0" priority="1" rank="10"/>
+    <cfRule type="top10" dxfId="5" priority="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Added in the first biome, added some animals to it as well
</commit_message>
<xml_diff>
--- a/research/Animals.xlsx
+++ b/research/Animals.xlsx
@@ -1,25 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
   <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JarvisWalker/Documents/Git/JSPets/research/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="1920" windowWidth="23085" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="1440" windowWidth="23080" windowHeight="12640" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -304,7 +309,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -472,11 +477,21 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF9C5700"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -547,16 +562,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -865,14 +870,14 @@
       <selection pane="bottomRight" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="6" max="6" width="4.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.83203125" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="6" max="6" width="4.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -916,7 +921,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -937,7 +942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -958,7 +963,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -976,7 +981,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1000,7 +1005,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1024,7 +1029,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1045,7 +1050,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1066,7 +1071,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1081,7 +1086,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1102,7 +1107,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1123,7 +1128,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1144,7 +1149,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1168,7 +1173,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1186,7 +1191,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1207,7 +1212,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1225,7 +1230,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1246,7 +1251,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1270,7 +1275,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1294,7 +1299,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>67</v>
       </c>
@@ -1345,12 +1350,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B19">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="lessThan">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="top10" dxfId="2" priority="1" rank="5"/>
+    <cfRule type="top10" dxfId="12" priority="1" rank="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -1362,22 +1367,22 @@
   <dimension ref="A1:AC48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="L3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N3" sqref="N3"/>
+      <selection pane="bottomRight" activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="14" max="14" width="11.7109375" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" customWidth="1"/>
-    <col min="16" max="16" width="14.42578125" customWidth="1"/>
+    <col min="1" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" customWidth="1"/>
+    <col min="14" max="14" width="11.6640625" customWidth="1"/>
+    <col min="15" max="15" width="12.83203125" customWidth="1"/>
+    <col min="16" max="16" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="E1" s="6" t="s">
         <v>84</v>
       </c>
@@ -1412,7 +1417,7 @@
       <c r="Z1" s="4"/>
       <c r="AA1" s="4"/>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -1495,7 +1500,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1528,12 +1533,12 @@
         <v>18</v>
       </c>
       <c r="L3">
-        <f>I3*F3*D3</f>
-        <v>8</v>
+        <f>I3+(F3*D3)</f>
+        <v>6</v>
       </c>
       <c r="M3">
-        <f>(J3+G3)*D3</f>
-        <v>4</v>
+        <f>J3+(G3*D3)</f>
+        <v>3</v>
       </c>
       <c r="R3">
         <v>10</v>
@@ -1548,7 +1553,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -1578,18 +1583,18 @@
         <v>30</v>
       </c>
       <c r="L4">
-        <f t="shared" ref="L4:L37" si="1">I4*F4*D4</f>
-        <v>0</v>
+        <f t="shared" ref="L4:L37" si="1">I4+(F4*D4)</f>
+        <v>2</v>
       </c>
       <c r="M4">
-        <f t="shared" ref="M4:M37" si="2">(J4+G4)*D4</f>
-        <v>4</v>
+        <f t="shared" ref="M4:M37" si="2">J4+(G4*D4)</f>
+        <v>3</v>
       </c>
       <c r="T4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -1620,17 +1625,17 @@
       </c>
       <c r="L5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M5">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U5">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -1661,11 +1666,11 @@
       </c>
       <c r="L6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M6">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="S6">
         <v>10</v>
@@ -1674,7 +1679,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -1705,17 +1710,17 @@
       </c>
       <c r="L7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M7">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y7">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -1749,11 +1754,11 @@
       </c>
       <c r="L8">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="M8">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N8">
         <v>3</v>
@@ -1765,7 +1770,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>43</v>
       </c>
@@ -1796,14 +1801,14 @@
       </c>
       <c r="L9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M9">
         <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -1834,14 +1839,14 @@
       </c>
       <c r="L10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M10">
         <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -1872,11 +1877,11 @@
       </c>
       <c r="L11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M11">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R11">
         <v>2</v>
@@ -1891,7 +1896,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -1922,11 +1927,11 @@
       </c>
       <c r="L12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M12">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="S12">
         <v>8</v>
@@ -1941,7 +1946,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -1972,11 +1977,11 @@
       </c>
       <c r="L13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M13">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="R13">
         <v>1</v>
@@ -1991,7 +1996,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -2022,11 +2027,11 @@
       </c>
       <c r="L14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M14">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S14">
         <v>10</v>
@@ -2038,7 +2043,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>38</v>
       </c>
@@ -2070,10 +2075,10 @@
       </c>
       <c r="M15">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -2087,14 +2092,17 @@
         <v>1</v>
       </c>
       <c r="F16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16">
         <v>12</v>
       </c>
+      <c r="I16">
+        <v>5</v>
+      </c>
       <c r="J16">
         <v>1</v>
       </c>
@@ -2104,11 +2112,11 @@
       </c>
       <c r="L16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="M16">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="Q16">
         <v>8</v>
@@ -2117,7 +2125,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -2148,11 +2156,11 @@
       </c>
       <c r="L17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M17">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R17">
         <v>10</v>
@@ -2173,7 +2181,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -2190,7 +2198,7 @@
         <v>1</v>
       </c>
       <c r="G18">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H18">
         <v>10</v>
@@ -2204,17 +2212,17 @@
       </c>
       <c r="L18">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M18">
         <f t="shared" si="2"/>
-        <v>4.5</v>
+        <v>1</v>
       </c>
       <c r="AA18">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -2245,17 +2253,17 @@
       </c>
       <c r="L19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M19">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="T19">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>46</v>
       </c>
@@ -2269,14 +2277,17 @@
         <v>1</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H20">
         <v>6</v>
       </c>
+      <c r="I20">
+        <v>5</v>
+      </c>
       <c r="J20">
         <v>1</v>
       </c>
@@ -2286,11 +2297,11 @@
       </c>
       <c r="L20">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="M20">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q20">
         <v>4</v>
@@ -2299,7 +2310,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>47</v>
       </c>
@@ -2313,28 +2324,31 @@
         <v>1</v>
       </c>
       <c r="F21">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G21">
         <v>1</v>
       </c>
       <c r="H21">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="I21">
+        <v>3</v>
       </c>
       <c r="J21">
         <v>1</v>
       </c>
       <c r="K21">
         <f t="shared" si="0"/>
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="L21">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="M21">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Q21">
         <v>10</v>
@@ -2349,7 +2363,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>48</v>
       </c>
@@ -2363,7 +2377,7 @@
         <v>1</v>
       </c>
       <c r="F22">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -2383,11 +2397,11 @@
       </c>
       <c r="L22">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="M22">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="N22">
         <v>4</v>
@@ -2405,7 +2419,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>49</v>
       </c>
@@ -2437,10 +2451,10 @@
       </c>
       <c r="M23">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>50</v>
       </c>
@@ -2471,11 +2485,11 @@
       </c>
       <c r="L24">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M24">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Q24" t="s">
         <v>85</v>
@@ -2511,7 +2525,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>51</v>
       </c>
@@ -2542,17 +2556,17 @@
       </c>
       <c r="L25">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M25">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Q25" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>52</v>
       </c>
@@ -2583,11 +2597,11 @@
       </c>
       <c r="L26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M26">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="R26">
         <v>10</v>
@@ -2599,7 +2613,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>53</v>
       </c>
@@ -2630,11 +2644,11 @@
       </c>
       <c r="L27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M27">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="S27">
         <v>5</v>
@@ -2649,7 +2663,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -2680,11 +2694,11 @@
       </c>
       <c r="L28">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M28">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="S28">
         <v>10</v>
@@ -2696,7 +2710,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>55</v>
       </c>
@@ -2727,11 +2741,11 @@
       </c>
       <c r="L29">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M29">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="S29">
         <v>10</v>
@@ -2749,7 +2763,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>56</v>
       </c>
@@ -2780,11 +2794,11 @@
       </c>
       <c r="L30">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M30">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="S30">
         <v>3</v>
@@ -2796,7 +2810,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>57</v>
       </c>
@@ -2827,17 +2841,17 @@
       </c>
       <c r="L31">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M31">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T31">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>58</v>
       </c>
@@ -2868,11 +2882,11 @@
       </c>
       <c r="L32">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M32">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="U32">
         <v>10</v>
@@ -2881,7 +2895,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>74</v>
       </c>
@@ -2912,11 +2926,11 @@
       </c>
       <c r="L33">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M33">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S33">
         <v>3</v>
@@ -2928,7 +2942,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>59</v>
       </c>
@@ -2959,11 +2973,11 @@
       </c>
       <c r="L34">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M34">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="V34">
         <v>10</v>
@@ -2972,7 +2986,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>79</v>
       </c>
@@ -3003,7 +3017,7 @@
       </c>
       <c r="L35">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M35">
         <f t="shared" si="2"/>
@@ -3013,7 +3027,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>80</v>
       </c>
@@ -3047,7 +3061,7 @@
       </c>
       <c r="L36">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M36">
         <f t="shared" si="2"/>
@@ -3060,7 +3074,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>82</v>
       </c>
@@ -3068,40 +3082,43 @@
         <v>81</v>
       </c>
       <c r="D37">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E37">
         <v>1</v>
       </c>
       <c r="F37">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H37">
         <v>20</v>
       </c>
+      <c r="I37">
+        <v>4</v>
+      </c>
       <c r="J37">
         <v>1</v>
       </c>
       <c r="K37">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="L37">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="M37">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q37">
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>67</v>
       </c>
@@ -3150,7 +3167,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.2">
       <c r="Q41">
         <f>SUM(Q3:Q39)</f>
         <v>30</v>
@@ -3199,37 +3216,37 @@
         <v>86</v>
       </c>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.2">
       <c r="Q43">
         <f>Q37/Q41</f>
         <v>0.1</v>
       </c>
     </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:29" x14ac:dyDescent="0.2">
       <c r="Q44">
         <f>Q22/Q41</f>
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.2">
       <c r="Q45">
         <f>Q21/Q41</f>
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.2">
       <c r="Q46">
         <f>Q20/Q41</f>
         <v>0.13333333333333333</v>
       </c>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.2">
       <c r="Q47">
         <f>Q16/Q41</f>
         <v>0.26666666666666666</v>
       </c>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:29" x14ac:dyDescent="0.2">
       <c r="Q48">
         <f xml:space="preserve"> SUM(Q43:Q47)</f>
         <v>1</v>
@@ -3237,25 +3254,25 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="top10" dxfId="13" priority="3" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="12" priority="10" rank="10"/>
+    <cfRule type="top10" dxfId="11" priority="3" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="10" priority="10" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="top10" dxfId="11" priority="9" rank="10"/>
+    <cfRule type="top10" dxfId="9" priority="9" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="top10" dxfId="10" priority="4" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="9" priority="7" rank="10"/>
+    <cfRule type="top10" dxfId="8" priority="4" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="7" priority="7" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="top10" dxfId="8" priority="6" rank="10"/>
-    <cfRule type="top10" dxfId="7" priority="2" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="6" priority="6" rank="10"/>
+    <cfRule type="top10" dxfId="5" priority="2" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:P1048576">
-    <cfRule type="top10" dxfId="6" priority="5" rank="10"/>
+    <cfRule type="top10" dxfId="4" priority="5" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="top10" dxfId="5" priority="1" rank="10"/>
+    <cfRule type="top10" dxfId="3" priority="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated the code so that it can load in a random animal with a random stage with each stage having a 'difficulty' which affects the spawned animal
</commit_message>
<xml_diff>
--- a/research/Animals.xlsx
+++ b/research/Animals.xlsx
@@ -1,30 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
   <workbookPr filterPrivacy="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JarvisWalker/Documents/Git/JSPets/research/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="1440" windowWidth="23080" windowHeight="12640" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="1440" windowWidth="23085" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -312,7 +307,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -836,21 +831,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K2" sqref="K2"/>
+      <selection pane="bottomRight" activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" customWidth="1"/>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
-    <col min="6" max="6" width="4.83203125" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="4.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -894,7 +889,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -912,10 +907,10 @@
         <v>10</v>
       </c>
       <c r="N2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -933,10 +928,10 @@
         <v>30</v>
       </c>
       <c r="N3">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -951,10 +946,10 @@
         <v>40</v>
       </c>
       <c r="N4">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -975,10 +970,10 @@
         <v>40</v>
       </c>
       <c r="N5">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -999,10 +994,10 @@
         <v>40</v>
       </c>
       <c r="N6">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1020,10 +1015,10 @@
         <v>50</v>
       </c>
       <c r="N7">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1041,10 +1036,10 @@
         <v>30</v>
       </c>
       <c r="N8">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1056,10 +1051,10 @@
         <v>100</v>
       </c>
       <c r="N9">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1077,10 +1072,10 @@
         <v>60</v>
       </c>
       <c r="N10">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1098,10 +1093,10 @@
         <v>50</v>
       </c>
       <c r="N11">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1119,10 +1114,10 @@
         <v>10</v>
       </c>
       <c r="N12">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1143,10 +1138,10 @@
         <v>30</v>
       </c>
       <c r="N13">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1161,10 +1156,10 @@
         <v>50</v>
       </c>
       <c r="N14">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1182,10 +1177,10 @@
         <v>20</v>
       </c>
       <c r="N15">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1200,10 +1195,10 @@
         <v>50</v>
       </c>
       <c r="N16">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1221,10 +1216,10 @@
         <v>60</v>
       </c>
       <c r="N17">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1245,10 +1240,10 @@
         <v>30</v>
       </c>
       <c r="N18">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1269,10 +1264,10 @@
         <v>20</v>
       </c>
       <c r="N19">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>67</v>
       </c>
@@ -1339,23 +1334,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="17.5" customWidth="1"/>
-    <col min="3" max="3" width="16.1640625" customWidth="1"/>
-    <col min="14" max="14" width="11.6640625" customWidth="1"/>
-    <col min="15" max="15" width="12.83203125" customWidth="1"/>
-    <col min="16" max="16" width="14.5" customWidth="1"/>
+    <col min="1" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E1" s="6" t="s">
         <v>84</v>
       </c>
@@ -1390,7 +1385,7 @@
       <c r="Z1" s="4"/>
       <c r="AA1" s="4"/>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -1473,7 +1468,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1526,7 +1521,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -1567,7 +1562,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -1608,7 +1603,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -1652,7 +1647,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -1693,7 +1688,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -1743,7 +1738,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>43</v>
       </c>
@@ -1781,7 +1776,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -1819,7 +1814,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -1869,7 +1864,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -1919,7 +1914,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -1969,7 +1964,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -2016,7 +2011,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>38</v>
       </c>
@@ -2051,7 +2046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -2098,7 +2093,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -2154,7 +2149,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -2195,7 +2190,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -2236,7 +2231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>46</v>
       </c>
@@ -2283,7 +2278,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>47</v>
       </c>
@@ -2336,7 +2331,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>48</v>
       </c>
@@ -2392,7 +2387,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>49</v>
       </c>
@@ -2427,7 +2422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>50</v>
       </c>
@@ -2498,7 +2493,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>51</v>
       </c>
@@ -2539,7 +2534,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>52</v>
       </c>
@@ -2586,7 +2581,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>53</v>
       </c>
@@ -2636,7 +2631,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -2683,7 +2678,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>55</v>
       </c>
@@ -2736,7 +2731,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>56</v>
       </c>
@@ -2783,7 +2778,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>57</v>
       </c>
@@ -2824,7 +2819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>58</v>
       </c>
@@ -2868,7 +2863,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>74</v>
       </c>
@@ -2915,7 +2910,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>59</v>
       </c>
@@ -2959,7 +2954,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>79</v>
       </c>
@@ -3000,7 +2995,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>80</v>
       </c>
@@ -3047,7 +3042,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>82</v>
       </c>
@@ -3091,7 +3086,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>91</v>
       </c>
@@ -3102,7 +3097,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>67</v>
       </c>
@@ -3151,7 +3146,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
       <c r="Q41">
         <f>SUM(Q3:Q39)</f>
         <v>30</v>
@@ -3200,37 +3195,37 @@
         <v>86</v>
       </c>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
       <c r="Q43">
         <f>Q37/Q41</f>
         <v>0.1</v>
       </c>
     </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:29" x14ac:dyDescent="0.25">
       <c r="Q44">
         <f>Q22/Q41</f>
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.25">
       <c r="Q45">
         <f>Q21/Q41</f>
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
       <c r="Q46">
         <f>Q20/Q41</f>
         <v>0.13333333333333333</v>
       </c>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
       <c r="Q47">
         <f>Q16/Q41</f>
         <v>0.26666666666666666</v>
       </c>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:29" x14ac:dyDescent="0.25">
       <c r="Q48">
         <f xml:space="preserve"> SUM(Q43:Q47)</f>
         <v>1</v>

</xml_diff>

<commit_message>
Updated some code to clean up various bugs
</commit_message>
<xml_diff>
--- a/research/Animals.xlsx
+++ b/research/Animals.xlsx
@@ -1,37 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
   <workbookPr filterPrivacy="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JarvisWalker/Documents/Git/JSPets/research/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="1440" windowWidth="23080" windowHeight="12640" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="1440" windowWidth="23085" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="92">
   <si>
     <t>City</t>
   </si>
@@ -304,12 +299,15 @@
   </si>
   <si>
     <t>Frog</t>
+  </si>
+  <si>
+    <t>Steps</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -851,500 +849,561 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P15" sqref="P15"/>
+      <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" customWidth="1"/>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
-    <col min="6" max="6" width="4.83203125" customWidth="1"/>
+    <col min="1" max="2" width="17.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="7" max="7" width="4.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" t="s">
         <v>65</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>22</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>23</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>86</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>24</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>85</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>25</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>87</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>26</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <f>SUM(C2:M2)</f>
+        <v>200</v>
+      </c>
+      <c r="C2">
+        <f>SUM(D2:N2)</f>
         <v>100</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>50</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>40</v>
       </c>
-      <c r="K2">
-        <v>10</v>
-      </c>
-      <c r="N2">
+      <c r="L2">
+        <v>10</v>
+      </c>
+      <c r="O2">
         <v>-5</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B19" si="0">SUM(C3:M3)</f>
+        <v>350</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C19" si="0">SUM(D3:N3)</f>
         <v>100</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>30</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>40</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>30</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>-3</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
+        <v>644</v>
+      </c>
+      <c r="C4">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>60</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>40</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>-2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
+        <v>570</v>
+      </c>
+      <c r="C5">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>30</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>20</v>
       </c>
-      <c r="J5">
-        <v>10</v>
-      </c>
-      <c r="M5">
+      <c r="K5">
+        <v>10</v>
+      </c>
+      <c r="N5">
         <v>40</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6">
+        <v>596</v>
+      </c>
+      <c r="C6">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="J6">
-        <v>10</v>
-      </c>
       <c r="K6">
         <v>10</v>
       </c>
       <c r="L6">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="M6">
         <v>40</v>
       </c>
       <c r="N6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="O6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7">
+        <v>500</v>
+      </c>
+      <c r="C7">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>40</v>
       </c>
-      <c r="K7">
-        <v>10</v>
-      </c>
-      <c r="M7">
+      <c r="L7">
+        <v>10</v>
+      </c>
+      <c r="N7">
         <v>50</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8">
+        <v>1160</v>
+      </c>
+      <c r="C8">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>40</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>30</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>30</v>
       </c>
-      <c r="N8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9">
+        <v>714</v>
+      </c>
+      <c r="C9">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>100</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10">
+        <v>916</v>
+      </c>
+      <c r="C10">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>30</v>
       </c>
-      <c r="I10">
-        <v>10</v>
-      </c>
-      <c r="K10">
+      <c r="J10">
+        <v>10</v>
+      </c>
+      <c r="L10">
         <v>60</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11">
+        <v>633</v>
+      </c>
+      <c r="C11">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>40</v>
       </c>
-      <c r="K11">
-        <v>10</v>
-      </c>
-      <c r="M11">
+      <c r="L11">
+        <v>10</v>
+      </c>
+      <c r="N11">
         <v>50</v>
       </c>
-      <c r="N11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12">
+        <v>1070</v>
+      </c>
+      <c r="C12">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>60</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>30</v>
       </c>
-      <c r="M12">
-        <v>10</v>
-      </c>
       <c r="N12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="O12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13">
+        <v>577</v>
+      </c>
+      <c r="C13">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>40</v>
       </c>
-      <c r="J13">
-        <v>10</v>
-      </c>
       <c r="K13">
+        <v>10</v>
+      </c>
+      <c r="L13">
         <v>20</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>30</v>
       </c>
-      <c r="N13">
+      <c r="O13">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14">
+        <v>231</v>
+      </c>
+      <c r="C14">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>50</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>50</v>
       </c>
-      <c r="N14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15">
+        <v>975</v>
+      </c>
+      <c r="C15">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>70</v>
       </c>
-      <c r="G15">
-        <v>10</v>
-      </c>
-      <c r="M15">
+      <c r="H15">
+        <v>10</v>
+      </c>
+      <c r="N15">
         <v>20</v>
       </c>
-      <c r="N15">
+      <c r="O15">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16">
+        <v>1040</v>
+      </c>
+      <c r="C16">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>50</v>
       </c>
-      <c r="L16">
+      <c r="M16">
         <v>50</v>
       </c>
-      <c r="N16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17">
+        <v>768</v>
+      </c>
+      <c r="C17">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>30</v>
       </c>
-      <c r="K17">
-        <v>10</v>
-      </c>
-      <c r="M17">
+      <c r="L17">
+        <v>10</v>
+      </c>
+      <c r="N17">
         <v>60</v>
       </c>
-      <c r="N17">
+      <c r="O17">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="B18">
+        <v>659</v>
+      </c>
+      <c r="C18">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="C18">
+      <c r="D18">
         <v>20</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>30</v>
       </c>
-      <c r="K18">
+      <c r="L18">
         <v>20</v>
       </c>
-      <c r="M18">
+      <c r="N18">
         <v>30</v>
       </c>
-      <c r="N18">
+      <c r="O18">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="B19">
+        <v>852</v>
+      </c>
+      <c r="C19">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>40</v>
       </c>
-      <c r="F19">
-        <v>10</v>
-      </c>
-      <c r="H19">
+      <c r="G19">
+        <v>10</v>
+      </c>
+      <c r="I19">
         <v>30</v>
       </c>
-      <c r="M19">
+      <c r="N19">
         <v>20</v>
       </c>
-      <c r="N19">
+      <c r="O19">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>66</v>
       </c>
-      <c r="C20">
-        <f>COUNTA(C2:C19)</f>
-        <v>3</v>
+      <c r="B20">
+        <f>SUM(B2:B19)</f>
+        <v>12455</v>
       </c>
       <c r="D20">
-        <f t="shared" ref="D20:M20" si="1">COUNTA(D2:D19)</f>
+        <f>COUNTA(D2:D19)</f>
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <f t="shared" ref="E20:N20" si="1">COUNTA(E2:E19)</f>
         <v>9</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="F20">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
       <c r="G20">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H20">
         <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="I20">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
       <c r="J20">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="K20">
         <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="L20">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
       <c r="M20">
         <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B19">
+  <conditionalFormatting sqref="C2:C19">
     <cfRule type="cellIs" dxfId="12" priority="2" operator="lessThan">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N1:N1048576">
+  <conditionalFormatting sqref="O1:O1048576">
     <cfRule type="top10" dxfId="11" priority="1" rank="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1356,24 +1415,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" zoomScalePageLayoutView="98" workbookViewId="0">
+    <sheetView zoomScale="98" zoomScaleNormal="98" zoomScalePageLayoutView="98" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="17.5" customWidth="1"/>
-    <col min="3" max="4" width="16.1640625" customWidth="1"/>
-    <col min="6" max="8" width="8.83203125" customWidth="1"/>
-    <col min="15" max="15" width="11.6640625" customWidth="1"/>
-    <col min="16" max="16" width="12.83203125" customWidth="1"/>
-    <col min="17" max="17" width="14.5" customWidth="1"/>
+    <col min="1" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="4" width="16.140625" customWidth="1"/>
+    <col min="6" max="8" width="8.85546875" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F1" s="6" t="s">
         <v>82</v>
       </c>
@@ -1408,7 +1467,7 @@
       <c r="AA1" s="4"/>
       <c r="AB1" s="4"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -1494,7 +1553,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -1502,11 +1561,11 @@
         <v>68</v>
       </c>
       <c r="C3" t="str">
-        <f>CONCATENATE(I3,"|",J3,"|",K3,"|",O3,"|",P3)</f>
+        <f t="shared" ref="C3:C38" si="0">CONCATENATE(I3,"|",J3,"|",K3,"|",O3,"|",P3)</f>
         <v>6|6|1||</v>
       </c>
       <c r="D3" t="str">
-        <f>CONCATENATE(L3,"|",M3,"|",N3,"|",O3,"|",P3)</f>
+        <f t="shared" ref="D3:D38" si="1">CONCATENATE(L3,"|",M3,"|",N3,"|",O3,"|",P3)</f>
         <v>12|8|3||</v>
       </c>
       <c r="E3">
@@ -1531,15 +1590,15 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <f>I3*E3*F3</f>
+        <f t="shared" ref="L3:L38" si="2">I3*E3*F3</f>
         <v>12</v>
       </c>
       <c r="M3">
-        <f>J3+(G3*E3)</f>
+        <f t="shared" ref="M3:M38" si="3">J3+(G3*E3)</f>
         <v>8</v>
       </c>
       <c r="N3">
-        <f>K3+(H3*E3)</f>
+        <f t="shared" ref="N3:N38" si="4">K3+(H3*E3)</f>
         <v>3</v>
       </c>
       <c r="T3">
@@ -1552,7 +1611,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>89</v>
       </c>
@@ -1560,11 +1619,11 @@
         <v>72</v>
       </c>
       <c r="C4" t="str">
-        <f>CONCATENATE(I4,"|",J4,"|",K4,"|",O4,"|",P4)</f>
+        <f t="shared" si="0"/>
         <v>7|5|1||</v>
       </c>
       <c r="D4" t="str">
-        <f>CONCATENATE(L4,"|",M4,"|",N4,"|",O4,"|",P4)</f>
+        <f t="shared" si="1"/>
         <v>21|8|4||</v>
       </c>
       <c r="E4">
@@ -1589,15 +1648,15 @@
         <v>1</v>
       </c>
       <c r="L4">
-        <f>I4*E4*F4</f>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="M4">
-        <f>J4+(G4*E4)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="N4">
-        <f>K4+(H4*E4)</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="T4">
@@ -1607,7 +1666,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -1615,11 +1674,11 @@
         <v>72</v>
       </c>
       <c r="C5" t="str">
-        <f>CONCATENATE(I5,"|",J5,"|",K5,"|",O5,"|",P5)</f>
+        <f t="shared" si="0"/>
         <v>8|4|1||10</v>
       </c>
       <c r="D5" t="str">
-        <f>CONCATENATE(L5,"|",M5,"|",N5,"|",O5,"|",P5)</f>
+        <f t="shared" si="1"/>
         <v>24|7|4||10</v>
       </c>
       <c r="E5">
@@ -1644,15 +1703,15 @@
         <v>1</v>
       </c>
       <c r="L5">
-        <f>I5*E5*F5</f>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="M5">
-        <f>J5+(G5*E5)</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="N5">
-        <f>K5+(H5*E5)</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="P5">
@@ -1665,7 +1724,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -1673,11 +1732,11 @@
         <v>69</v>
       </c>
       <c r="C6" t="str">
-        <f>CONCATENATE(I6,"|",J6,"|",K6,"|",O6,"|",P6)</f>
+        <f t="shared" si="0"/>
         <v>8|5|1||</v>
       </c>
       <c r="D6" t="str">
-        <f>CONCATENATE(L6,"|",M6,"|",N6,"|",O6,"|",P6)</f>
+        <f t="shared" si="1"/>
         <v>24|8|4||</v>
       </c>
       <c r="E6">
@@ -1702,15 +1761,15 @@
         <v>1</v>
       </c>
       <c r="L6">
-        <f>I6*E6*F6</f>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="M6">
-        <f>J6+(G6*E6)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="N6">
-        <f>K6+(H6*E6)</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="T6">
@@ -1726,7 +1785,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>56</v>
       </c>
@@ -1734,11 +1793,11 @@
         <v>71</v>
       </c>
       <c r="C7" t="str">
-        <f>CONCATENATE(I7,"|",J7,"|",K7,"|",O7,"|",P7)</f>
+        <f t="shared" si="0"/>
         <v>16|12|0||</v>
       </c>
       <c r="D7" t="str">
-        <f>CONCATENATE(L7,"|",M7,"|",N7,"|",O7,"|",P7)</f>
+        <f t="shared" si="1"/>
         <v>32|14|2||</v>
       </c>
       <c r="E7">
@@ -1763,22 +1822,22 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <f>I7*E7*F7</f>
+        <f t="shared" si="2"/>
         <v>32</v>
       </c>
       <c r="M7">
-        <f>J7+(G7*E7)</f>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="N7">
-        <f>K7+(H7*E7)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="U7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -1786,11 +1845,11 @@
         <v>69</v>
       </c>
       <c r="C8" t="str">
-        <f>CONCATENATE(I8,"|",J8,"|",K8,"|",O8,"|",P8)</f>
+        <f t="shared" si="0"/>
         <v>8|4|1|4|7</v>
       </c>
       <c r="D8" t="str">
-        <f>CONCATENATE(L8,"|",M8,"|",N8,"|",O8,"|",P8)</f>
+        <f t="shared" si="1"/>
         <v>24|16|4|4|7</v>
       </c>
       <c r="E8">
@@ -1815,15 +1874,15 @@
         <v>1</v>
       </c>
       <c r="L8">
-        <f>I8*E8*F8</f>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="M8">
-        <f>J8+(G8*E8)</f>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="N8">
-        <f>K8+(H8*E8)</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="O8">
@@ -1842,7 +1901,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>43</v>
       </c>
@@ -1850,11 +1909,11 @@
         <v>68</v>
       </c>
       <c r="C9" t="str">
-        <f>CONCATENATE(I9,"|",J9,"|",K9,"|",O9,"|",P9)</f>
+        <f t="shared" si="0"/>
         <v>8||1||</v>
       </c>
       <c r="D9" t="str">
-        <f>CONCATENATE(L9,"|",M9,"|",N9,"|",O9,"|",P9)</f>
+        <f t="shared" si="1"/>
         <v>16|2|3||</v>
       </c>
       <c r="E9">
@@ -1876,19 +1935,19 @@
         <v>1</v>
       </c>
       <c r="L9">
-        <f>I9*E9*F9</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="M9">
-        <f>J9+(G9*E9)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="N9">
-        <f>K9+(H9*E9)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -1896,11 +1955,11 @@
         <v>68</v>
       </c>
       <c r="C10" t="str">
-        <f>CONCATENATE(I10,"|",J10,"|",K10,"|",O10,"|",P10)</f>
+        <f t="shared" si="0"/>
         <v>10||1||</v>
       </c>
       <c r="D10" t="str">
-        <f>CONCATENATE(L10,"|",M10,"|",N10,"|",O10,"|",P10)</f>
+        <f t="shared" si="1"/>
         <v>20|2|3||</v>
       </c>
       <c r="E10">
@@ -1922,19 +1981,19 @@
         <v>1</v>
       </c>
       <c r="L10">
-        <f>I10*E10*F10</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="M10">
-        <f>J10+(G10*E10)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="N10">
-        <f>K10+(H10*E10)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -1942,11 +2001,11 @@
         <v>68</v>
       </c>
       <c r="C11" t="str">
-        <f>CONCATENATE(I11,"|",J11,"|",K11,"|",O11,"|",P11)</f>
+        <f t="shared" si="0"/>
         <v>8|6|1||</v>
       </c>
       <c r="D11" t="str">
-        <f>CONCATENATE(L11,"|",M11,"|",N11,"|",O11,"|",P11)</f>
+        <f t="shared" si="1"/>
         <v>16|8|3||</v>
       </c>
       <c r="E11">
@@ -1971,15 +2030,15 @@
         <v>1</v>
       </c>
       <c r="L11">
-        <f>I11*E11*F11</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="M11">
-        <f>J11+(G11*E11)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="N11">
-        <f>K11+(H11*E11)</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="T11">
@@ -1995,7 +2054,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -2003,11 +2062,11 @@
         <v>68</v>
       </c>
       <c r="C12" t="str">
-        <f>CONCATENATE(I12,"|",J12,"|",K12,"|",O12,"|",P12)</f>
+        <f t="shared" si="0"/>
         <v>10|4|1||</v>
       </c>
       <c r="D12" t="str">
-        <f>CONCATENATE(L12,"|",M12,"|",N12,"|",O12,"|",P12)</f>
+        <f t="shared" si="1"/>
         <v>30|7|1||</v>
       </c>
       <c r="E12">
@@ -2032,22 +2091,22 @@
         <v>1</v>
       </c>
       <c r="L12">
-        <f>I12*E12*F12</f>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="M12">
-        <f>J12+(G12*E12)</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="N12">
-        <f>K12+(H12*E12)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AB12">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -2055,11 +2114,11 @@
         <v>68</v>
       </c>
       <c r="C13" t="str">
-        <f>CONCATENATE(I13,"|",J13,"|",K13,"|",O13,"|",P13)</f>
+        <f t="shared" si="0"/>
         <v>8|8|1||</v>
       </c>
       <c r="D13" t="str">
-        <f>CONCATENATE(L13,"|",M13,"|",N13,"|",O13,"|",P13)</f>
+        <f t="shared" si="1"/>
         <v>16|10|3||</v>
       </c>
       <c r="E13">
@@ -2084,22 +2143,22 @@
         <v>1</v>
       </c>
       <c r="L13">
-        <f>I13*E13*F13</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="M13">
-        <f>J13+(G13*E13)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="N13">
-        <f>K13+(H13*E13)</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="U13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>90</v>
       </c>
@@ -2107,11 +2166,11 @@
         <v>70</v>
       </c>
       <c r="C14" t="str">
-        <f>CONCATENATE(I14,"|",J14,"|",K14,"|",O14,"|",P14)</f>
+        <f t="shared" si="0"/>
         <v>5|5|1||</v>
       </c>
       <c r="D14" t="str">
-        <f>CONCATENATE(L14,"|",M14,"|",N14,"|",O14,"|",P14)</f>
+        <f t="shared" si="1"/>
         <v>15|11|7||</v>
       </c>
       <c r="E14">
@@ -2136,15 +2195,15 @@
         <v>1</v>
       </c>
       <c r="L14">
-        <f>I14*E14*F14</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="M14">
-        <f>J14+(G14*E14)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="N14">
-        <f>K14+(H14*E14)</f>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="T14">
@@ -2157,7 +2216,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>38</v>
       </c>
@@ -2165,11 +2224,11 @@
         <v>68</v>
       </c>
       <c r="C15" t="str">
-        <f>CONCATENATE(I15,"|",J15,"|",K15,"|",O15,"|",P15)</f>
+        <f t="shared" si="0"/>
         <v>8||1||</v>
       </c>
       <c r="D15" t="str">
-        <f>CONCATENATE(L15,"|",M15,"|",N15,"|",O15,"|",P15)</f>
+        <f t="shared" si="1"/>
         <v>0|0|1||</v>
       </c>
       <c r="F15">
@@ -2188,19 +2247,19 @@
         <v>1</v>
       </c>
       <c r="L15">
-        <f>I15*E15*F15</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M15">
-        <f>J15+(G15*E15)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N15">
-        <f>K15+(H15*E15)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -2208,11 +2267,11 @@
         <v>68</v>
       </c>
       <c r="C16" t="str">
-        <f>CONCATENATE(I16,"|",J16,"|",K16,"|",O16,"|",P16)</f>
+        <f t="shared" si="0"/>
         <v>9|6|1|3|6</v>
       </c>
       <c r="D16" t="str">
-        <f>CONCATENATE(L16,"|",M16,"|",N16,"|",O16,"|",P16)</f>
+        <f t="shared" si="1"/>
         <v>18|8|3|3|6</v>
       </c>
       <c r="E16">
@@ -2237,15 +2296,15 @@
         <v>1</v>
       </c>
       <c r="L16">
-        <f>I16*E16*F16</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="M16">
-        <f>J16+(G16*E16)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="N16">
-        <f>K16+(H16*E16)</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="O16">
@@ -2258,7 +2317,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -2266,11 +2325,11 @@
         <v>68</v>
       </c>
       <c r="C17" t="str">
-        <f>CONCATENATE(I17,"|",J17,"|",K17,"|",O17,"|",P17)</f>
+        <f t="shared" si="0"/>
         <v>7|7|1||</v>
       </c>
       <c r="D17" t="str">
-        <f>CONCATENATE(L17,"|",M17,"|",N17,"|",O17,"|",P17)</f>
+        <f t="shared" si="1"/>
         <v>14|13|3||</v>
       </c>
       <c r="E17">
@@ -2295,22 +2354,22 @@
         <v>1</v>
       </c>
       <c r="L17">
-        <f>I17*E17*F17</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="M17">
-        <f>J17+(G17*E17)</f>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="N17">
-        <f>K17+(H17*E17)</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="Z17">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -2318,11 +2377,11 @@
         <v>68</v>
       </c>
       <c r="C18" t="str">
-        <f>CONCATENATE(I18,"|",J18,"|",K18,"|",O18,"|",P18)</f>
+        <f t="shared" si="0"/>
         <v>8|8|2||</v>
       </c>
       <c r="D18" t="str">
-        <f>CONCATENATE(L18,"|",M18,"|",N18,"|",O18,"|",P18)</f>
+        <f t="shared" si="1"/>
         <v>24|11|5||</v>
       </c>
       <c r="E18">
@@ -2347,15 +2406,15 @@
         <v>2</v>
       </c>
       <c r="L18">
-        <f>I18*E18*F18</f>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="M18">
-        <f>J18+(G18*E18)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="N18">
-        <f>K18+(H18*E18)</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="T18">
@@ -2365,7 +2424,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>79</v>
       </c>
@@ -2373,11 +2432,11 @@
         <v>80</v>
       </c>
       <c r="C19" t="str">
-        <f>CONCATENATE(I19,"|",J19,"|",K19,"|",O19,"|",P19)</f>
+        <f t="shared" si="0"/>
         <v>80|10|1|5|</v>
       </c>
       <c r="D19" t="str">
-        <f>CONCATENATE(L19,"|",M19,"|",N19,"|",O19,"|",P19)</f>
+        <f t="shared" si="1"/>
         <v>80|10|1|5|</v>
       </c>
       <c r="E19">
@@ -2402,15 +2461,15 @@
         <v>1</v>
       </c>
       <c r="L19">
-        <f>I19*E19*F19</f>
+        <f t="shared" si="2"/>
         <v>80</v>
       </c>
       <c r="M19">
-        <f>J19+(G19*E19)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="N19">
-        <f>K19+(H19*E19)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="O19">
@@ -2420,7 +2479,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>55</v>
       </c>
@@ -2428,11 +2487,11 @@
         <v>69</v>
       </c>
       <c r="C20" t="str">
-        <f>CONCATENATE(I20,"|",J20,"|",K20,"|",O20,"|",P20)</f>
+        <f t="shared" si="0"/>
         <v>9|5|1|2|8</v>
       </c>
       <c r="D20" t="str">
-        <f>CONCATENATE(L20,"|",M20,"|",N20,"|",O20,"|",P20)</f>
+        <f t="shared" si="1"/>
         <v>27|8|4|2|8</v>
       </c>
       <c r="E20">
@@ -2457,15 +2516,15 @@
         <v>1</v>
       </c>
       <c r="L20">
-        <f>I20*E20*F20</f>
+        <f t="shared" si="2"/>
         <v>27</v>
       </c>
       <c r="M20">
-        <f>J20+(G20*E20)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="N20">
-        <f>K20+(H20*E20)</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="O20">
@@ -2490,7 +2549,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>52</v>
       </c>
@@ -2498,11 +2557,11 @@
         <v>69</v>
       </c>
       <c r="C21" t="str">
-        <f>CONCATENATE(I21,"|",J21,"|",K21,"|",O21,"|",P21)</f>
+        <f t="shared" si="0"/>
         <v>7|6|1||</v>
       </c>
       <c r="D21" t="str">
-        <f>CONCATENATE(L21,"|",M21,"|",N21,"|",O21,"|",P21)</f>
+        <f t="shared" si="1"/>
         <v>21|9|4||</v>
       </c>
       <c r="E21">
@@ -2527,15 +2586,15 @@
         <v>1</v>
       </c>
       <c r="L21">
-        <f>I21*E21*F21</f>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="M21">
-        <f>J21+(G21*E21)</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="N21">
-        <f>K21+(H21*E21)</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="S21">
@@ -2548,7 +2607,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>54</v>
       </c>
@@ -2556,11 +2615,11 @@
         <v>69</v>
       </c>
       <c r="C22" t="str">
-        <f>CONCATENATE(I22,"|",J22,"|",K22,"|",O22,"|",P22)</f>
+        <f t="shared" si="0"/>
         <v>9|5|1|6|2</v>
       </c>
       <c r="D22" t="str">
-        <f>CONCATENATE(L22,"|",M22,"|",N22,"|",O22,"|",P22)</f>
+        <f t="shared" si="1"/>
         <v>27|8|1|6|2</v>
       </c>
       <c r="E22">
@@ -2585,15 +2644,15 @@
         <v>1</v>
       </c>
       <c r="L22">
-        <f>I22*E22*F22</f>
+        <f t="shared" si="2"/>
         <v>27</v>
       </c>
       <c r="M22">
-        <f>J22+(G22*E22)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="N22">
-        <f>K22+(H22*E22)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="O22">
@@ -2612,7 +2671,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>49</v>
       </c>
@@ -2620,11 +2679,11 @@
         <v>69</v>
       </c>
       <c r="C23" t="str">
-        <f>CONCATENATE(I23,"|",J23,"|",K23,"|",O23,"|",P23)</f>
+        <f t="shared" si="0"/>
         <v>8||1||</v>
       </c>
       <c r="D23" t="str">
-        <f>CONCATENATE(L23,"|",M23,"|",N23,"|",O23,"|",P23)</f>
+        <f t="shared" si="1"/>
         <v>0|0|1||</v>
       </c>
       <c r="F23">
@@ -2643,19 +2702,19 @@
         <v>1</v>
       </c>
       <c r="L23">
-        <f>I23*E23*F23</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M23">
-        <f>J23+(G23*E23)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N23">
-        <f>K23+(H23*E23)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>50</v>
       </c>
@@ -2663,11 +2722,11 @@
         <v>69</v>
       </c>
       <c r="C24" t="str">
-        <f>CONCATENATE(I24,"|",J24,"|",K24,"|",O24,"|",P24)</f>
+        <f t="shared" si="0"/>
         <v>7||1||</v>
       </c>
       <c r="D24" t="str">
-        <f>CONCATENATE(L24,"|",M24,"|",N24,"|",O24,"|",P24)</f>
+        <f t="shared" si="1"/>
         <v>21|3|4||</v>
       </c>
       <c r="E24">
@@ -2689,15 +2748,15 @@
         <v>1</v>
       </c>
       <c r="L24">
-        <f>I24*E24*F24</f>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="M24">
-        <f>J24+(G24*E24)</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="N24">
-        <f>K24+(H24*E24)</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="R24" t="s">
@@ -2734,7 +2793,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="25" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>51</v>
       </c>
@@ -2742,11 +2801,11 @@
         <v>69</v>
       </c>
       <c r="C25" t="str">
-        <f>CONCATENATE(I25,"|",J25,"|",K25,"|",O25,"|",P25)</f>
+        <f t="shared" si="0"/>
         <v>8||1||</v>
       </c>
       <c r="D25" t="str">
-        <f>CONCATENATE(L25,"|",M25,"|",N25,"|",O25,"|",P25)</f>
+        <f t="shared" si="1"/>
         <v>24|3|4||</v>
       </c>
       <c r="E25">
@@ -2768,22 +2827,22 @@
         <v>1</v>
       </c>
       <c r="L25">
-        <f>I25*E25*F25</f>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="M25">
-        <f>J25+(G25*E25)</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="N25">
-        <f>K25+(H25*E25)</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="R25" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>47</v>
       </c>
@@ -2791,11 +2850,11 @@
         <v>69</v>
       </c>
       <c r="C26" t="str">
-        <f>CONCATENATE(I26,"|",J26,"|",K26,"|",O26,"|",P26)</f>
+        <f t="shared" si="0"/>
         <v>12|6|1||</v>
       </c>
       <c r="D26" t="str">
-        <f>CONCATENATE(L26,"|",M26,"|",N26,"|",O26,"|",P26)</f>
+        <f t="shared" si="1"/>
         <v>36|9|4||</v>
       </c>
       <c r="E26">
@@ -2820,15 +2879,15 @@
         <v>1</v>
       </c>
       <c r="L26">
-        <f>I26*E26*F26</f>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="M26">
-        <f>J26+(G26*E26)</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="N26">
-        <f>K26+(H26*E26)</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="R26">
@@ -2844,7 +2903,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>46</v>
       </c>
@@ -2852,11 +2911,11 @@
         <v>69</v>
       </c>
       <c r="C27" t="str">
-        <f>CONCATENATE(I27,"|",J27,"|",K27,"|",O27,"|",P27)</f>
+        <f t="shared" si="0"/>
         <v>6|5|1||</v>
       </c>
       <c r="D27" t="str">
-        <f>CONCATENATE(L27,"|",M27,"|",N27,"|",O27,"|",P27)</f>
+        <f t="shared" si="1"/>
         <v>18|14|7||</v>
       </c>
       <c r="E27">
@@ -2881,15 +2940,15 @@
         <v>1</v>
       </c>
       <c r="L27">
-        <f>I27*E27*F27</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="M27">
-        <f>J27+(G27*E27)</f>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="N27">
-        <f>K27+(H27*E27)</f>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="R27">
@@ -2899,7 +2958,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -2907,11 +2966,11 @@
         <v>68</v>
       </c>
       <c r="C28" t="str">
-        <f>CONCATENATE(I28,"|",J28,"|",K28,"|",O28,"|",P28)</f>
+        <f t="shared" si="0"/>
         <v>8|7|1||</v>
       </c>
       <c r="D28" t="str">
-        <f>CONCATENATE(L28,"|",M28,"|",N28,"|",O28,"|",P28)</f>
+        <f t="shared" si="1"/>
         <v>16|9|3||</v>
       </c>
       <c r="E28">
@@ -2936,15 +2995,15 @@
         <v>1</v>
       </c>
       <c r="L28">
-        <f>I28*E28*F28</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="M28">
-        <f>J28+(G28*E28)</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="N28">
-        <f>K28+(H28*E28)</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="S28">
@@ -2960,7 +3019,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -2968,11 +3027,11 @@
         <v>68</v>
       </c>
       <c r="C29" t="str">
-        <f>CONCATENATE(I29,"|",J29,"|",K29,"|",O29,"|",P29)</f>
+        <f t="shared" si="0"/>
         <v>8|3|1||</v>
       </c>
       <c r="D29" t="str">
-        <f>CONCATENATE(L29,"|",M29,"|",N29,"|",O29,"|",P29)</f>
+        <f t="shared" si="1"/>
         <v>16|5|3||</v>
       </c>
       <c r="E29">
@@ -2997,15 +3056,15 @@
         <v>1</v>
       </c>
       <c r="L29">
-        <f>I29*E29*F29</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="M29">
-        <f>J29+(G29*E29)</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="N29">
-        <f>K29+(H29*E29)</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="S29">
@@ -3027,7 +3086,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>81</v>
       </c>
@@ -3035,11 +3094,11 @@
         <v>80</v>
       </c>
       <c r="C30" t="str">
-        <f>CONCATENATE(I30,"|",J30,"|",K30,"|",O30,"|",P30)</f>
+        <f t="shared" si="0"/>
         <v>20|4|1||</v>
       </c>
       <c r="D30" t="str">
-        <f>CONCATENATE(L30,"|",M30,"|",N30,"|",O30,"|",P30)</f>
+        <f t="shared" si="1"/>
         <v>60|13|1||</v>
       </c>
       <c r="E30">
@@ -3064,22 +3123,22 @@
         <v>1</v>
       </c>
       <c r="L30">
-        <f>I30*E30*F30</f>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
       <c r="M30">
-        <f>J30+(G30*E30)</f>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="N30">
-        <f>K30+(H30*E30)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="R30">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -3087,11 +3146,11 @@
         <v>68</v>
       </c>
       <c r="C31" t="str">
-        <f>CONCATENATE(I31,"|",J31,"|",K31,"|",O31,"|",P31)</f>
+        <f t="shared" si="0"/>
         <v>12|5|1||</v>
       </c>
       <c r="D31" t="str">
-        <f>CONCATENATE(L31,"|",M31,"|",N31,"|",O31,"|",P31)</f>
+        <f t="shared" si="1"/>
         <v>36|11|1||</v>
       </c>
       <c r="E31">
@@ -3116,15 +3175,15 @@
         <v>1</v>
       </c>
       <c r="L31">
-        <f>I31*E31*F31</f>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="M31">
-        <f>J31+(G31*E31)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="N31">
-        <f>K31+(H31*E31)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="R31">
@@ -3134,7 +3193,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>73</v>
       </c>
@@ -3142,11 +3201,11 @@
         <v>71</v>
       </c>
       <c r="C32" t="str">
-        <f>CONCATENATE(I32,"|",J32,"|",K32,"|",O32,"|",P32)</f>
+        <f t="shared" si="0"/>
         <v>8|10|1||</v>
       </c>
       <c r="D32" t="str">
-        <f>CONCATENATE(L32,"|",M32,"|",N32,"|",O32,"|",P32)</f>
+        <f t="shared" si="1"/>
         <v>16|12|3||</v>
       </c>
       <c r="E32">
@@ -3171,15 +3230,15 @@
         <v>1</v>
       </c>
       <c r="L32">
-        <f>I32*E32*F32</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="M32">
-        <f>J32+(G32*E32)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="N32">
-        <f>K32+(H32*E32)</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="T32">
@@ -3192,7 +3251,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>78</v>
       </c>
@@ -3200,11 +3259,11 @@
         <v>80</v>
       </c>
       <c r="C33" t="str">
-        <f>CONCATENATE(I33,"|",J33,"|",K33,"|",O33,"|",P33)</f>
+        <f t="shared" si="0"/>
         <v>36|12|1||</v>
       </c>
       <c r="D33" t="str">
-        <f>CONCATENATE(L33,"|",M33,"|",N33,"|",O33,"|",P33)</f>
+        <f t="shared" si="1"/>
         <v>36|12|1||</v>
       </c>
       <c r="E33">
@@ -3229,22 +3288,22 @@
         <v>1</v>
       </c>
       <c r="L33">
-        <f>I33*E33*F33</f>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="M33">
-        <f>J33+(G33*E33)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="N33">
-        <f>K33+(H33*E33)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="Y33">
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>28</v>
       </c>
@@ -3252,11 +3311,11 @@
         <v>68</v>
       </c>
       <c r="C34" t="str">
-        <f>CONCATENATE(I34,"|",J34,"|",K34,"|",O34,"|",P34)</f>
+        <f t="shared" si="0"/>
         <v>9|4|1||</v>
       </c>
       <c r="D34" t="str">
-        <f>CONCATENATE(L34,"|",M34,"|",N34,"|",O34,"|",P34)</f>
+        <f t="shared" si="1"/>
         <v>18|6|3||</v>
       </c>
       <c r="E34">
@@ -3281,15 +3340,15 @@
         <v>1</v>
       </c>
       <c r="L34">
-        <f>I34*E34*F34</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="M34">
-        <f>J34+(G34*E34)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="N34">
-        <f>K34+(H34*E34)</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="S34">
@@ -3305,7 +3364,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>29</v>
       </c>
@@ -3313,11 +3372,11 @@
         <v>68</v>
       </c>
       <c r="C35" t="str">
-        <f>CONCATENATE(I35,"|",J35,"|",K35,"|",O35,"|",P35)</f>
+        <f t="shared" si="0"/>
         <v>15|15|1||</v>
       </c>
       <c r="D35" t="str">
-        <f>CONCATENATE(L35,"|",M35,"|",N35,"|",O35,"|",P35)</f>
+        <f t="shared" si="1"/>
         <v>30|17|3||</v>
       </c>
       <c r="E35">
@@ -3342,22 +3401,22 @@
         <v>1</v>
       </c>
       <c r="L35">
-        <f>I35*E35*F35</f>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="M35">
-        <f>J35+(G35*E35)</f>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="N35">
-        <f>K35+(H35*E35)</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="U35">
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>57</v>
       </c>
@@ -3365,11 +3424,11 @@
         <v>71</v>
       </c>
       <c r="C36" t="str">
-        <f>CONCATENATE(I36,"|",J36,"|",K36,"|",O36,"|",P36)</f>
+        <f t="shared" si="0"/>
         <v>12|3|1||</v>
       </c>
       <c r="D36" t="str">
-        <f>CONCATENATE(L36,"|",M36,"|",N36,"|",O36,"|",P36)</f>
+        <f t="shared" si="1"/>
         <v>36|6|4||</v>
       </c>
       <c r="E36">
@@ -3394,15 +3453,15 @@
         <v>1</v>
       </c>
       <c r="L36">
-        <f>I36*E36*F36</f>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="M36">
-        <f>J36+(G36*E36)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="N36">
-        <f>K36+(H36*E36)</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="V36">
@@ -3412,7 +3471,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>30</v>
       </c>
@@ -3420,11 +3479,11 @@
         <v>68</v>
       </c>
       <c r="C37" t="str">
-        <f>CONCATENATE(I37,"|",J37,"|",K37,"|",O37,"|",P37)</f>
+        <f t="shared" si="0"/>
         <v>36|15|1||</v>
       </c>
       <c r="D37" t="str">
-        <f>CONCATENATE(L37,"|",M37,"|",N37,"|",O37,"|",P37)</f>
+        <f t="shared" si="1"/>
         <v>72|17|1||</v>
       </c>
       <c r="E37">
@@ -3449,22 +3508,22 @@
         <v>1</v>
       </c>
       <c r="L37">
-        <f>I37*E37*F37</f>
+        <f t="shared" si="2"/>
         <v>72</v>
       </c>
       <c r="M37">
-        <f>J37+(G37*E37)</f>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="N37">
-        <f>K37+(H37*E37)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="V37">
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -3472,11 +3531,11 @@
         <v>68</v>
       </c>
       <c r="C38" t="str">
-        <f>CONCATENATE(I38,"|",J38,"|",K38,"|",O38,"|",P38)</f>
+        <f t="shared" si="0"/>
         <v>7|8|1||</v>
       </c>
       <c r="D38" t="str">
-        <f>CONCATENATE(L38,"|",M38,"|",N38,"|",O38,"|",P38)</f>
+        <f t="shared" si="1"/>
         <v>21|11|4||</v>
       </c>
       <c r="E38">
@@ -3501,15 +3560,15 @@
         <v>1</v>
       </c>
       <c r="L38">
-        <f>I38*E38*F38</f>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="M38">
-        <f>J38+(G38*E38)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="N38">
-        <f>K38+(H38*E38)</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="S38">
@@ -3525,98 +3584,98 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>66</v>
       </c>
       <c r="R40">
-        <f t="shared" ref="R40:AB40" si="0">COUNT(R3:R39)</f>
+        <f t="shared" ref="R40:AB40" si="5">COUNT(R3:R39)</f>
         <v>5</v>
       </c>
       <c r="S40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="T40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
       <c r="U40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="V40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="W40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="X40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="Y40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="Z40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="AA40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="AB40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:30" x14ac:dyDescent="0.25">
       <c r="R41">
-        <f t="shared" ref="R41:AB41" si="1">SUM(R3:R39)</f>
+        <f t="shared" ref="R41:AB41" si="6">SUM(R3:R39)</f>
         <v>30</v>
       </c>
       <c r="S41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>57</v>
       </c>
       <c r="T41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>105</v>
       </c>
       <c r="U41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="V41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>38</v>
       </c>
       <c r="W41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>72</v>
       </c>
       <c r="X41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>22</v>
       </c>
       <c r="Y41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>21</v>
       </c>
       <c r="Z41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>60</v>
       </c>
       <c r="AA41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>56</v>
       </c>
       <c r="AB41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>63</v>
       </c>
       <c r="AD41" t="s">

</xml_diff>

<commit_message>
Old work that I had been working on but forgot to commit
</commit_message>
<xml_diff>
--- a/research/Animals.xlsx
+++ b/research/Animals.xlsx
@@ -1,32 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
   <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JarvisWalker/Documents/Git/JSPets/research/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="1440" windowWidth="23085" windowHeight="12645"/>
+    <workbookView xWindow="600" yWindow="1440" windowWidth="23080" windowHeight="12640" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="95">
   <si>
     <t>City</t>
   </si>
@@ -302,12 +307,21 @@
   </si>
   <si>
     <t>Steps</t>
+  </si>
+  <si>
+    <t>UnlockCondition</t>
+  </si>
+  <si>
+    <t>isUnlocked</t>
+  </si>
+  <si>
+    <t>Appearance</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -442,7 +456,167 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="28">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -560,16 +734,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -851,21 +1015,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomRight" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="17.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="7" max="7" width="4.85546875" customWidth="1"/>
+    <col min="1" max="2" width="17.83203125" customWidth="1"/>
+    <col min="3" max="3" width="16.5" customWidth="1"/>
+    <col min="7" max="7" width="4.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -912,7 +1076,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -936,7 +1100,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -960,7 +1124,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -981,7 +1145,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1008,7 +1172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1035,7 +1199,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1059,7 +1223,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1083,7 +1247,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1101,7 +1265,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1125,7 +1289,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1149,7 +1313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1173,7 +1337,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1200,7 +1364,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1221,7 +1385,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1245,7 +1409,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1266,7 +1430,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1290,7 +1454,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1317,7 +1481,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1344,7 +1508,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>66</v>
       </c>
@@ -1399,12 +1563,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C19">
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="lessThan">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="top10" dxfId="11" priority="1" rank="5"/>
+    <cfRule type="top10" dxfId="12" priority="1" rank="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -1413,26 +1577,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD41"/>
+  <dimension ref="A1:AG41"/>
   <sheetViews>
-    <sheetView zoomScale="98" zoomScaleNormal="98" zoomScalePageLayoutView="98" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" zoomScalePageLayoutView="98" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="O3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C27" sqref="C27"/>
+      <selection pane="bottomRight" activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="4" width="16.140625" customWidth="1"/>
-    <col min="6" max="8" width="8.85546875" customWidth="1"/>
-    <col min="15" max="15" width="11.7109375" customWidth="1"/>
-    <col min="16" max="16" width="12.85546875" customWidth="1"/>
-    <col min="17" max="17" width="14.42578125" customWidth="1"/>
+    <col min="1" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="4" width="16.1640625" customWidth="1"/>
+    <col min="6" max="8" width="8.83203125" customWidth="1"/>
+    <col min="15" max="15" width="11.6640625" customWidth="1"/>
+    <col min="16" max="16" width="12.83203125" customWidth="1"/>
+    <col min="17" max="20" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="F1" s="6" t="s">
         <v>82</v>
       </c>
@@ -1453,12 +1617,12 @@
       </c>
       <c r="P1" s="5"/>
       <c r="Q1" s="5"/>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
       <c r="V1" s="4"/>
       <c r="W1" s="4"/>
       <c r="X1" s="4"/>
@@ -1466,8 +1630,11 @@
       <c r="Z1" s="4"/>
       <c r="AA1" s="4"/>
       <c r="AB1" s="4"/>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC1" s="4"/>
+      <c r="AD1" s="4"/>
+      <c r="AE1" s="4"/>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -1520,40 +1687,49 @@
         <v>77</v>
       </c>
       <c r="R2" t="s">
+        <v>93</v>
+      </c>
+      <c r="S2" t="s">
+        <v>92</v>
+      </c>
+      <c r="T2" t="s">
+        <v>94</v>
+      </c>
+      <c r="U2" t="s">
         <v>19</v>
       </c>
-      <c r="S2" t="s">
+      <c r="V2" t="s">
         <v>20</v>
       </c>
-      <c r="T2" t="s">
+      <c r="W2" t="s">
         <v>21</v>
       </c>
-      <c r="U2" t="s">
+      <c r="X2" t="s">
         <v>22</v>
       </c>
-      <c r="V2" t="s">
+      <c r="Y2" t="s">
         <v>23</v>
       </c>
-      <c r="W2" t="s">
+      <c r="Z2" t="s">
         <v>86</v>
       </c>
-      <c r="X2" t="s">
+      <c r="AA2" t="s">
         <v>24</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="AB2" t="s">
         <v>85</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AC2" t="s">
         <v>25</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AD2" t="s">
         <v>87</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AE2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -1601,17 +1777,27 @@
         <f t="shared" ref="N3:N38" si="4">K3+(H3*E3)</f>
         <v>3</v>
       </c>
+      <c r="R3" t="b">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>5</v>
+      </c>
       <c r="T3">
-        <v>10</v>
-      </c>
-      <c r="X3">
-        <v>3</v>
-      </c>
-      <c r="Z3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+        <f>SUM(U3:AE3)</f>
+        <v>16</v>
+      </c>
+      <c r="W3">
+        <v>10</v>
+      </c>
+      <c r="AA3">
+        <v>3</v>
+      </c>
+      <c r="AC3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>89</v>
       </c>
@@ -1659,14 +1845,24 @@
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
+      <c r="R4" t="b">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>6</v>
+      </c>
       <c r="T4">
-        <v>8</v>
+        <f t="shared" ref="T4:T38" si="5">SUM(U4:AE4)</f>
+        <v>18</v>
       </c>
       <c r="W4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="Z4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -1717,14 +1913,24 @@
       <c r="P5">
         <v>10</v>
       </c>
-      <c r="W5">
-        <v>10</v>
-      </c>
-      <c r="AA5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="R5" t="b">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>6</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="Z5">
+        <v>10</v>
+      </c>
+      <c r="AD5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -1772,20 +1978,30 @@
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
+      <c r="R6" t="b">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>8</v>
+      </c>
       <c r="T6">
+        <f t="shared" si="5"/>
+        <v>35</v>
+      </c>
+      <c r="W6">
         <v>5</v>
       </c>
-      <c r="W6">
-        <v>10</v>
-      </c>
       <c r="Z6">
         <v>10</v>
       </c>
-      <c r="AA6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC6">
+        <v>10</v>
+      </c>
+      <c r="AD6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>56</v>
       </c>
@@ -1833,11 +2049,21 @@
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="U7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="R7" t="b">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>5</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="X7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -1891,17 +2117,27 @@
       <c r="P8">
         <v>7</v>
       </c>
-      <c r="R8">
+      <c r="R8" t="b">
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="5"/>
+        <v>25</v>
+      </c>
+      <c r="U8">
         <v>5</v>
       </c>
-      <c r="V8">
-        <v>10</v>
-      </c>
-      <c r="AB8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Y8">
+        <v>10</v>
+      </c>
+      <c r="AE8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>43</v>
       </c>
@@ -1946,8 +2182,15 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+      <c r="R9" t="b">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -1992,8 +2235,15 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="R10" t="b">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -2041,20 +2291,30 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="R11" t="b">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>8</v>
+      </c>
       <c r="T11">
-        <v>8</v>
+        <f t="shared" si="5"/>
+        <v>25</v>
       </c>
       <c r="W11">
+        <v>8</v>
+      </c>
+      <c r="Z11">
         <v>6</v>
       </c>
-      <c r="X11">
-        <v>3</v>
-      </c>
-      <c r="Y11">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AA11">
+        <v>3</v>
+      </c>
+      <c r="AB11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -2102,11 +2362,21 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="AB12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="R12" t="b">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>5</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="AE12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -2154,11 +2424,21 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="U13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="R13" t="b">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>4</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="X13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>90</v>
       </c>
@@ -2206,17 +2486,27 @@
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
+      <c r="R14" t="b">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>6</v>
+      </c>
       <c r="T14">
-        <v>3</v>
-      </c>
-      <c r="X14">
-        <v>3</v>
-      </c>
-      <c r="Y14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="W14">
+        <v>3</v>
+      </c>
+      <c r="AA14">
+        <v>3</v>
+      </c>
+      <c r="AB14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>38</v>
       </c>
@@ -2258,8 +2548,15 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="R15" t="b">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -2313,11 +2610,21 @@
       <c r="P16">
         <v>6</v>
       </c>
-      <c r="Z16">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="R16" t="b">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>6</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="AC16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -2365,11 +2672,21 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="Z17">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="R17" t="b">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>6</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="AC17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -2417,14 +2734,24 @@
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
+      <c r="R18" t="b">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>5</v>
+      </c>
       <c r="T18">
-        <v>10</v>
+        <f t="shared" si="5"/>
+        <v>18</v>
       </c>
       <c r="W18">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="Z18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>79</v>
       </c>
@@ -2475,11 +2802,21 @@
       <c r="O19">
         <v>5</v>
       </c>
-      <c r="X19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="R19" t="b">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>5</v>
+      </c>
+      <c r="T19">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="AA19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>55</v>
       </c>
@@ -2533,23 +2870,33 @@
       <c r="P20">
         <v>8</v>
       </c>
+      <c r="R20" t="b">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>8</v>
+      </c>
       <c r="T20">
-        <v>10</v>
+        <f t="shared" si="5"/>
+        <v>31</v>
       </c>
       <c r="W20">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="Z20">
         <v>5</v>
       </c>
-      <c r="AA20">
-        <v>8</v>
-      </c>
-      <c r="AB20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC20">
+        <v>5</v>
+      </c>
+      <c r="AD20">
+        <v>8</v>
+      </c>
+      <c r="AE20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>52</v>
       </c>
@@ -2597,17 +2944,27 @@
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
+      <c r="R21" t="b">
+        <v>0</v>
+      </c>
       <c r="S21">
-        <v>10</v>
-      </c>
-      <c r="Z21">
-        <v>10</v>
-      </c>
-      <c r="AA21">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="T21">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="V21">
+        <v>10</v>
+      </c>
+      <c r="AC21">
+        <v>10</v>
+      </c>
+      <c r="AD21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>54</v>
       </c>
@@ -2661,17 +3018,27 @@
       <c r="P22">
         <v>2</v>
       </c>
+      <c r="R22" t="b">
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <v>7</v>
+      </c>
       <c r="T22">
-        <v>10</v>
+        <f t="shared" si="5"/>
+        <v>20</v>
       </c>
       <c r="W22">
+        <v>10</v>
+      </c>
+      <c r="Z22">
         <v>5</v>
       </c>
-      <c r="AA22">
+      <c r="AD22">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>49</v>
       </c>
@@ -2713,8 +3080,15 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+      <c r="R23" t="b">
+        <v>0</v>
+      </c>
+      <c r="T23">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>50</v>
       </c>
@@ -2759,14 +3133,12 @@
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="R24" t="s">
-        <v>83</v>
-      </c>
-      <c r="S24" t="s">
-        <v>83</v>
-      </c>
-      <c r="T24" t="s">
-        <v>83</v>
+      <c r="R24" t="b">
+        <v>0</v>
+      </c>
+      <c r="T24">
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="U24" t="s">
         <v>83</v>
@@ -2792,8 +3164,17 @@
       <c r="AB24" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="25" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+      <c r="AC24" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD24" t="s">
+        <v>83</v>
+      </c>
+      <c r="AE24" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>51</v>
       </c>
@@ -2838,11 +3219,18 @@
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="R25" t="s">
+      <c r="R25" t="b">
+        <v>0</v>
+      </c>
+      <c r="T25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="U25" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>47</v>
       </c>
@@ -2890,20 +3278,30 @@
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="R26">
-        <v>10</v>
+      <c r="R26" t="b">
+        <v>0</v>
       </c>
       <c r="S26">
+        <v>8</v>
+      </c>
+      <c r="T26">
+        <f t="shared" si="5"/>
+        <v>29</v>
+      </c>
+      <c r="U26">
         <v>10</v>
       </c>
       <c r="V26">
-        <v>3</v>
-      </c>
-      <c r="AB26">
+        <v>10</v>
+      </c>
+      <c r="Y26">
+        <v>3</v>
+      </c>
+      <c r="AE26">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>46</v>
       </c>
@@ -2951,14 +3349,24 @@
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="R27">
+      <c r="R27" t="b">
+        <v>0</v>
+      </c>
+      <c r="S27">
+        <v>8</v>
+      </c>
+      <c r="T27">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="U27">
         <v>4</v>
       </c>
-      <c r="S27">
+      <c r="V27">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -3006,20 +3414,30 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="R28" t="b">
+        <v>0</v>
+      </c>
       <c r="S28">
+        <v>6</v>
+      </c>
+      <c r="T28">
+        <f t="shared" si="5"/>
+        <v>32</v>
+      </c>
+      <c r="V28">
         <v>2</v>
       </c>
-      <c r="T28">
-        <v>10</v>
-      </c>
-      <c r="V28">
-        <v>10</v>
-      </c>
-      <c r="AB28">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="W28">
+        <v>10</v>
+      </c>
+      <c r="Y28">
+        <v>10</v>
+      </c>
+      <c r="AE28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -3067,26 +3485,36 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="R29" t="b">
+        <v>0</v>
+      </c>
       <c r="S29">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="T29">
-        <v>8</v>
+        <f t="shared" si="5"/>
+        <v>56</v>
+      </c>
+      <c r="V29">
+        <v>10</v>
       </c>
       <c r="W29">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="Z29">
         <v>10</v>
       </c>
-      <c r="AA29">
-        <v>10</v>
-      </c>
-      <c r="AB29">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC29">
+        <v>10</v>
+      </c>
+      <c r="AD29">
+        <v>10</v>
+      </c>
+      <c r="AE29">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>81</v>
       </c>
@@ -3134,11 +3562,21 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="R30">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="R30" t="b">
+        <v>0</v>
+      </c>
+      <c r="S30">
+        <v>5</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="U30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -3186,14 +3624,24 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="R31">
-        <v>8</v>
+      <c r="R31" t="b">
+        <v>0</v>
       </c>
       <c r="S31">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+      <c r="U31">
+        <v>8</v>
+      </c>
+      <c r="V31">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>73</v>
       </c>
@@ -3241,17 +3689,27 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="R32" t="b">
+        <v>0</v>
+      </c>
+      <c r="S32">
+        <v>8</v>
+      </c>
       <c r="T32">
-        <v>3</v>
-      </c>
-      <c r="AA32">
-        <v>3</v>
-      </c>
-      <c r="AB32">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="W32">
+        <v>3</v>
+      </c>
+      <c r="AD32">
+        <v>3</v>
+      </c>
+      <c r="AE32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>78</v>
       </c>
@@ -3299,11 +3757,21 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Y33">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="R33" t="b">
+        <v>0</v>
+      </c>
+      <c r="S33">
+        <v>10</v>
+      </c>
+      <c r="T33">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="AB33">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>28</v>
       </c>
@@ -3351,20 +3819,30 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
+      <c r="R34" t="b">
+        <v>0</v>
+      </c>
       <c r="S34">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="T34">
-        <v>10</v>
-      </c>
-      <c r="X34">
-        <v>10</v>
-      </c>
-      <c r="Z34">
+        <f t="shared" si="5"/>
+        <v>32</v>
+      </c>
+      <c r="V34">
+        <v>10</v>
+      </c>
+      <c r="W34">
+        <v>10</v>
+      </c>
+      <c r="AA34">
+        <v>10</v>
+      </c>
+      <c r="AC34">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>29</v>
       </c>
@@ -3412,11 +3890,21 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="U35">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="R35" t="b">
+        <v>0</v>
+      </c>
+      <c r="S35">
+        <v>5</v>
+      </c>
+      <c r="T35">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="X35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>57</v>
       </c>
@@ -3464,14 +3952,24 @@
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="V36">
-        <v>10</v>
-      </c>
-      <c r="AB36">
+      <c r="R36" t="b">
+        <v>0</v>
+      </c>
+      <c r="S36">
+        <v>8</v>
+      </c>
+      <c r="T36">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="Y36">
+        <v>10</v>
+      </c>
+      <c r="AE36">
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>30</v>
       </c>
@@ -3519,11 +4017,21 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="V37">
+      <c r="R37" t="b">
+        <v>0</v>
+      </c>
+      <c r="S37">
+        <v>3</v>
+      </c>
+      <c r="T37">
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="Y37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -3571,114 +4079,124 @@
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
+      <c r="R38" t="b">
+        <v>0</v>
+      </c>
       <c r="S38">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="T38">
-        <v>10</v>
+        <f t="shared" si="5"/>
+        <v>27</v>
+      </c>
+      <c r="V38">
+        <v>1</v>
       </c>
       <c r="W38">
-        <v>8</v>
-      </c>
-      <c r="AB38">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="Z38">
+        <v>8</v>
+      </c>
+      <c r="AE38">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>66</v>
       </c>
-      <c r="R40">
-        <f t="shared" ref="R40:AB40" si="5">COUNT(R3:R39)</f>
+      <c r="U40">
+        <f t="shared" ref="U40:AE40" si="6">COUNT(U3:U39)</f>
         <v>5</v>
       </c>
-      <c r="S40">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="T40">
-        <f t="shared" si="5"/>
+      <c r="V40">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="W40">
+        <f t="shared" si="6"/>
         <v>13</v>
       </c>
-      <c r="U40">
-        <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-      <c r="V40">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="W40">
-        <f t="shared" si="5"/>
-        <v>9</v>
-      </c>
       <c r="X40">
-        <f t="shared" si="5"/>
-        <v>5</v>
+        <f t="shared" si="6"/>
+        <v>3</v>
       </c>
       <c r="Y40">
-        <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-      <c r="Z40">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="AA40">
-        <f t="shared" si="5"/>
-        <v>7</v>
-      </c>
-      <c r="AB40">
-        <f t="shared" si="5"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="R41">
-        <f t="shared" ref="R41:AB41" si="6">SUM(R3:R39)</f>
-        <v>30</v>
-      </c>
-      <c r="S41">
-        <f t="shared" si="6"/>
-        <v>57</v>
-      </c>
-      <c r="T41">
-        <f t="shared" si="6"/>
-        <v>105</v>
-      </c>
-      <c r="U41">
         <f t="shared" si="6"/>
         <v>5</v>
       </c>
+      <c r="Z40">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="AA40">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="AB40">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="AC40">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="AD40">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="AE40">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="U41">
+        <f t="shared" ref="U41:AE41" si="7">SUM(U3:U39)</f>
+        <v>30</v>
+      </c>
       <c r="V41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
+        <v>57</v>
+      </c>
+      <c r="W41">
+        <f t="shared" si="7"/>
+        <v>105</v>
+      </c>
+      <c r="X41">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="Y41">
+        <f t="shared" si="7"/>
         <v>38</v>
       </c>
-      <c r="W41">
-        <f t="shared" si="6"/>
+      <c r="Z41">
+        <f t="shared" si="7"/>
         <v>72</v>
       </c>
-      <c r="X41">
-        <f t="shared" si="6"/>
+      <c r="AA41">
+        <f t="shared" si="7"/>
         <v>22</v>
       </c>
-      <c r="Y41">
-        <f t="shared" si="6"/>
+      <c r="AB41">
+        <f t="shared" si="7"/>
         <v>21</v>
       </c>
-      <c r="Z41">
-        <f t="shared" si="6"/>
+      <c r="AC41">
+        <f t="shared" si="7"/>
         <v>60</v>
       </c>
-      <c r="AA41">
-        <f t="shared" si="6"/>
+      <c r="AD41">
+        <f t="shared" si="7"/>
         <v>56</v>
       </c>
-      <c r="AB41">
-        <f t="shared" si="6"/>
+      <c r="AE41">
+        <f t="shared" si="7"/>
         <v>63</v>
       </c>
-      <c r="AD41" t="s">
+      <c r="AG41" t="s">
         <v>84</v>
       </c>
     </row>
@@ -3687,31 +4205,34 @@
     <sortCondition ref="A3"/>
   </sortState>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="top10" dxfId="10" priority="5" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="9" priority="12" rank="10"/>
+    <cfRule type="top10" dxfId="11" priority="7" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="10" priority="14" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="top10" dxfId="8" priority="11" rank="10"/>
+    <cfRule type="top10" dxfId="9" priority="13" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="top10" dxfId="7" priority="6" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="6" priority="9" rank="10"/>
+    <cfRule type="top10" dxfId="8" priority="8" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="7" priority="11" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:M1048576">
-    <cfRule type="top10" dxfId="5" priority="4" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="4" priority="8" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N1:Q1048576">
-    <cfRule type="top10" dxfId="3" priority="7" rank="10"/>
+    <cfRule type="top10" dxfId="6" priority="6" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="5" priority="10" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="top10" dxfId="2" priority="3" rank="10"/>
+    <cfRule type="top10" dxfId="4" priority="5" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C38">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T1:T1048576">
+    <cfRule type="top10" dxfId="1" priority="2" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S1:S1048576">
+    <cfRule type="top10" dxfId="0" priority="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>